<commit_message>
final thought exercises until more info from work
</commit_message>
<xml_diff>
--- a/Spreadsheets/Stock Options.xlsx
+++ b/Spreadsheets/Stock Options.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ISO" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="AMT" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="NQSO" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Scenarios" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="NQSO" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
   <si>
     <t xml:space="preserve">STOCK PRICE</t>
   </si>
@@ -187,6 +188,27 @@
   </si>
   <si>
     <t xml:space="preserve">28%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPO Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lock Out Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMT Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phased Out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONG-TERM CAPITAL</t>
   </si>
   <si>
     <t xml:space="preserve">ISO?</t>
@@ -230,7 +252,7 @@
     <numFmt numFmtId="179" formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0"/>
     <numFmt numFmtId="180" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -361,8 +383,15 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,6 +401,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF666666"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
         <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
@@ -448,7 +483,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="98">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -731,6 +766,62 @@
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="179" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -844,7 +935,7 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666666"/>
-      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF999999"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -866,7 +957,7 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1597,8 +1688,8 @@
   </sheetPr>
   <dimension ref="A2:G31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2005,6 +2096,399 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="1.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="1.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="9.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="56" t="n">
+        <v>12550</v>
+      </c>
+      <c r="C1" s="71"/>
+      <c r="D1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="56" t="n">
+        <f aca="false">B8-B1+E2</f>
+        <v>237450</v>
+      </c>
+      <c r="F1" s="72"/>
+      <c r="I1" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="73" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>73600</v>
+      </c>
+      <c r="C2" s="71"/>
+      <c r="D2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="56"/>
+      <c r="F2" s="72"/>
+      <c r="I2" s="56" t="n">
+        <f aca="false">MAX(0,E1-B18)*A19+MIN(B18-B17,MAX(0,E1-B17))*A18+MIN(B17-B16,MAX(0,E1-B16))*A17+MIN(B16-B15,MAX(0,E1-B15))*A16+MIN(B15-B14,MAX(0,E1-B14))*A15+MIN(B14-B13,MAX(0,E1-B13))*A14+MIN(B13,MAX(0,E1))*A13+MAX(0,IF(E4&gt;E13,(E4-E13)*D14, 0))+MAX(0,IF(E4&gt;B23,MIN((B24-B23),(E3-B23))*A24, 0))+MAX(0,IF(E4&gt;B24,(E3-B24)*A25, 0))</f>
+        <v>59074.85</v>
+      </c>
+      <c r="J2" s="66" t="n">
+        <f aca="false">I2/(E4)</f>
+        <v>0.248788587070962</v>
+      </c>
+      <c r="K2" s="56" t="n">
+        <f aca="false">MIN(E18,E8)*D18+MAX(0,IF(E8&gt;E18,(E8-E18)*D19, 0))</f>
+        <v>45864</v>
+      </c>
+      <c r="L2" s="66" t="n">
+        <f aca="false">K2/(E6)</f>
+        <v>0.183456</v>
+      </c>
+      <c r="M2" s="56" t="n">
+        <f aca="false">MAX(0,(I2-K2))/((D18+D19)/2)</f>
+        <v>48929.0740740741</v>
+      </c>
+      <c r="N2" s="56" t="n">
+        <f aca="false">MAX(0,(K2-I2))/0.35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>523600</v>
+      </c>
+      <c r="C3" s="71"/>
+      <c r="D3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="56"/>
+      <c r="F3" s="74"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="58" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="71"/>
+      <c r="D4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="56" t="n">
+        <f aca="false">E1+E3</f>
+        <v>237450</v>
+      </c>
+      <c r="F4" s="74"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="75" t="n">
+        <v>44378</v>
+      </c>
+      <c r="C5" s="71"/>
+      <c r="D5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="72"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>180</v>
+      </c>
+      <c r="C6" s="71"/>
+      <c r="D6" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="56" t="n">
+        <f aca="false">B8+E2+E3+E5</f>
+        <v>250000</v>
+      </c>
+      <c r="F6" s="72"/>
+      <c r="I6" s="57"/>
+      <c r="K6" s="57"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="75" t="n">
+        <f aca="false">B5+B6</f>
+        <v>44558</v>
+      </c>
+      <c r="C7" s="71"/>
+      <c r="D7" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="56" t="n">
+        <f aca="false">MIN(B2,MAX(0,B4*(E6-B3)))</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="72"/>
+      <c r="I7" s="56"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="73" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="76" t="n">
+        <v>250000</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="56" t="n">
+        <f aca="false">E6-B2+E7</f>
+        <v>176400</v>
+      </c>
+      <c r="F8" s="72"/>
+      <c r="I8" s="56"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="59"/>
+      <c r="F11" s="56"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="78"/>
+      <c r="D12" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="56"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="79" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="62" t="n">
+        <v>9950</v>
+      </c>
+      <c r="C13" s="80"/>
+      <c r="D13" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="62" t="n">
+        <v>200000</v>
+      </c>
+      <c r="F13" s="56"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="62" t="n">
+        <v>40525</v>
+      </c>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81" t="n">
+        <v>0.038</v>
+      </c>
+      <c r="F14" s="56"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="62" t="n">
+        <v>86375</v>
+      </c>
+      <c r="C15" s="80"/>
+      <c r="F15" s="56"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="62" t="n">
+        <v>164925</v>
+      </c>
+      <c r="C16" s="80"/>
+      <c r="D16" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="59"/>
+      <c r="F16" s="65"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="62" t="n">
+        <v>209425</v>
+      </c>
+      <c r="C17" s="80"/>
+      <c r="D17" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="66"/>
+      <c r="G17" s="57"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="62" t="n">
+        <v>523600</v>
+      </c>
+      <c r="C18" s="80"/>
+      <c r="D18" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="62" t="n">
+        <v>199900</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="79" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="79" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="63"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="82"/>
+      <c r="F22" s="56"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="83" t="n">
+        <v>0</v>
+      </c>
+      <c r="B23" s="62" t="n">
+        <v>40400</v>
+      </c>
+      <c r="C23" s="57"/>
+      <c r="F23" s="56"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="83" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="B24" s="63" t="n">
+        <v>445850</v>
+      </c>
+      <c r="C24" s="57"/>
+      <c r="F24" s="56"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="84" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="F25" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A21:B21"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:AD19"/>
@@ -2015,25 +2499,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="71" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="71" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="71" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="72" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="71" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="71" width="4.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="71" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="71" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="71" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="71" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="71" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="71" width="5.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="71" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="71" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="71" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="71" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="71" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="71" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="71" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="85" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="85" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="85" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="86" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="85" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="85" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="85" width="4.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="85" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="85" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="85" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="85" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="85" width="5.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="85" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="85" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="85" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="85" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="85" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="85" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="85" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2119,13 +2603,13 @@
         <v>5</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>7</v>
@@ -2137,10 +2621,10 @@
         <v>9</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="6" t="s">
@@ -2188,13 +2672,13 @@
       <c r="C4" s="11" t="n">
         <v>30000</v>
       </c>
-      <c r="D4" s="73" t="n">
+      <c r="D4" s="87" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="74" t="n">
+      <c r="F4" s="88" t="n">
         <f aca="false">DATEDIF(A4,C18,"Y")</f>
         <v>4</v>
       </c>
@@ -2209,7 +2693,7 @@
       <c r="I4" s="11" t="n">
         <v>30000</v>
       </c>
-      <c r="J4" s="75" t="n">
+      <c r="J4" s="89" t="n">
         <f aca="false">H4/C4</f>
         <v>1</v>
       </c>
@@ -2267,14 +2751,14 @@
       <c r="C5" s="11" t="n">
         <v>123519</v>
       </c>
-      <c r="D5" s="73" t="n">
+      <c r="D5" s="87" t="n">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="76" t="s">
-        <v>59</v>
+      <c r="F5" s="90" t="s">
+        <v>66</v>
       </c>
       <c r="G5" s="13" t="n">
         <f aca="false">MAX(0,MIN(36,DATEDIF(A5,C18,"M")))</f>
@@ -2287,7 +2771,7 @@
       <c r="I5" s="20" t="n">
         <v>83375</v>
       </c>
-      <c r="J5" s="75" t="n">
+      <c r="J5" s="89" t="n">
         <f aca="false">H5/C5</f>
         <v>0.675</v>
       </c>
@@ -2345,13 +2829,13 @@
       <c r="C6" s="11" t="n">
         <v>38380</v>
       </c>
-      <c r="D6" s="73" t="n">
+      <c r="D6" s="87" t="n">
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="74" t="n">
+      <c r="F6" s="88" t="n">
         <f aca="false">DATEDIF(A6,C18,"Y")</f>
         <v>1</v>
       </c>
@@ -2366,7 +2850,7 @@
       <c r="I6" s="20" t="n">
         <v>10394</v>
       </c>
-      <c r="J6" s="75" t="n">
+      <c r="J6" s="89" t="n">
         <f aca="false">H6/C6</f>
         <v>0.270833333333333</v>
       </c>
@@ -2424,13 +2908,13 @@
       <c r="C7" s="11" t="n">
         <v>138965</v>
       </c>
-      <c r="D7" s="73" t="n">
+      <c r="D7" s="87" t="n">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="74" t="n">
+      <c r="F7" s="88" t="n">
         <f aca="false">DATEDIF(A7,C18,"Y")</f>
         <v>0</v>
       </c>
@@ -2445,7 +2929,7 @@
       <c r="I7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="75" t="n">
+      <c r="J7" s="89" t="n">
         <f aca="false">H7/C7</f>
         <v>0</v>
       </c>
@@ -2498,9 +2982,9 @@
       <c r="A8" s="13"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="73"/>
+      <c r="D8" s="87"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="75"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="13"/>
       <c r="H8" s="14"/>
       <c r="I8" s="11"/>
@@ -2551,7 +3035,7 @@
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="77"/>
+      <c r="D9" s="91"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -2604,7 +3088,7 @@
       <c r="A10" s="30"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="77"/>
+      <c r="D10" s="91"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -2614,7 +3098,7 @@
       <c r="K10" s="13"/>
       <c r="L10" s="29"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="78"/>
+      <c r="N10" s="92"/>
       <c r="O10" s="13"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="17"/>
@@ -2636,7 +3120,7 @@
       <c r="A11" s="11"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="77"/>
+      <c r="D11" s="91"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -2668,7 +3152,7 @@
       <c r="A12" s="31"/>
       <c r="B12" s="30"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="77"/>
+      <c r="D12" s="91"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -2732,7 +3216,7 @@
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
-      <c r="D14" s="73"/>
+      <c r="D14" s="87"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -2764,7 +3248,7 @@
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
-      <c r="D15" s="73"/>
+      <c r="D15" s="87"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -2792,7 +3276,7 @@
       <c r="AC15" s="13"/>
       <c r="AD15" s="13"/>
     </row>
-    <row r="16" s="80" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="94" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="35" t="str">
         <f aca="false">"Grants: "&amp;COUNT(A4:A7)</f>
         <v>Grants: 4</v>
@@ -2802,7 +3286,7 @@
         <f aca="false">SUM(C4:C7)</f>
         <v>330864</v>
       </c>
-      <c r="D16" s="79"/>
+      <c r="D16" s="93"/>
       <c r="E16" s="37"/>
       <c r="F16" s="40"/>
       <c r="G16" s="38"/>
@@ -2844,13 +3328,13 @@
       <c r="AC16" s="38"/>
       <c r="AD16" s="38"/>
     </row>
-    <row r="17" s="83" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="97" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="44"/>
       <c r="B17" s="45"/>
       <c r="C17" s="46"/>
-      <c r="D17" s="81"/>
+      <c r="D17" s="95"/>
       <c r="E17" s="46"/>
-      <c r="F17" s="82"/>
+      <c r="F17" s="96"/>
       <c r="G17" s="47"/>
       <c r="H17" s="47"/>
       <c r="I17" s="47"/>
@@ -2891,7 +3375,7 @@
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="75"/>
+      <c r="F18" s="89"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
@@ -2928,7 +3412,7 @@
       <c r="C19" s="51"/>
       <c r="D19" s="51"/>
       <c r="E19" s="11"/>
-      <c r="F19" s="75"/>
+      <c r="F19" s="89"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
@@ -2936,7 +3420,7 @@
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="54" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="N19" s="54"/>
       <c r="O19" s="54"/>

</xml_diff>

<commit_message>
updated dividend + 401K
</commit_message>
<xml_diff>
--- a/Spreadsheets/Stock Options.xlsx
+++ b/Spreadsheets/Stock Options.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="1" state="visible" r:id="rId2"/>
@@ -800,7 +800,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="161">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -973,416 +973,412 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="13" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="13" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="178" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="179" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="180" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="179" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="180" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="182" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="183" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="177" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="13" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="174" fontId="13" fillId="0" borderId="17" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="177" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="179" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="180" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="179" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="180" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="182" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="183" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1532,7 +1528,7 @@
   </sheetPr>
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -1628,11 +1624,11 @@
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">IF($B$11&lt;E4, 203, 0)</f>
-        <v>203</v>
+        <v>0</v>
       </c>
       <c r="C4" s="10" t="n">
         <f aca="false">B4*$A$1</f>
-        <v>1827</v>
+        <v>0</v>
       </c>
       <c r="D4" s="11" t="n">
         <v>43831</v>
@@ -1734,18 +1730,18 @@
       </c>
       <c r="B10" s="14" t="n">
         <f aca="false">SUM(B4:B7)</f>
-        <v>540</v>
+        <v>337</v>
       </c>
       <c r="C10" s="15" t="n">
         <f aca="false">SUM(C4:C7)</f>
-        <v>4860</v>
+        <v>3033</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="16" t="n">
         <f aca="false">C10*12</f>
-        <v>58320</v>
+        <v>36396</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,7 +1750,7 @@
       </c>
       <c r="B11" s="18" t="n">
         <f aca="true">TODAY()</f>
-        <v>44538</v>
+        <v>44544</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,8 +2288,8 @@
   </sheetPr>
   <dimension ref="A2:T52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2398,7 +2394,7 @@
         <v>52</v>
       </c>
       <c r="I4" s="41" t="n">
-        <v>160000</v>
+        <v>153000</v>
       </c>
       <c r="K4" s="42" t="s">
         <v>51</v>
@@ -2459,10 +2455,10 @@
         <f aca="false">Schedule!H16+5000</f>
         <v>133169</v>
       </c>
-      <c r="S5" s="43" t="s">
+      <c r="S5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="43"/>
+      <c r="T5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="38" t="s">
@@ -2481,7 +2477,7 @@
       </c>
       <c r="I6" s="41" t="n">
         <f aca="false">I4+I5</f>
-        <v>160000</v>
+        <v>153000</v>
       </c>
       <c r="K6" s="42" t="s">
         <v>57</v>
@@ -2522,7 +2518,7 @@
       </c>
       <c r="F7" s="39" t="n">
         <f aca="false">MAX(0,IF((I$7-I$5)&gt;E6,MIN((E7-E6),((I$7-I$5)-E6))*D7, 0))</f>
-        <v>14658</v>
+        <v>12978</v>
       </c>
       <c r="G7" s="40"/>
       <c r="H7" s="0" t="s">
@@ -2530,7 +2526,7 @@
       </c>
       <c r="I7" s="41" t="n">
         <f aca="false">I6-$B$2</f>
-        <v>147450</v>
+        <v>140450</v>
       </c>
       <c r="K7" s="42" t="s">
         <v>61</v>
@@ -2552,7 +2548,7 @@
       <c r="S7" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="T7" s="44" t="n">
+      <c r="T7" s="43" t="n">
         <f aca="false">(1831+656+468)</f>
         <v>2955</v>
       </c>
@@ -2574,7 +2570,7 @@
       </c>
       <c r="I8" s="25" t="n">
         <f aca="false">SUM(F4:F10)</f>
-        <v>29409</v>
+        <v>27729</v>
       </c>
       <c r="K8" s="42" t="s">
         <v>63</v>
@@ -2615,7 +2611,7 @@
       <c r="H9" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="45" t="n">
+      <c r="I9" s="44" t="n">
         <f aca="false">SUM(F14:F16)+SUM(F20:F21)</f>
         <v>0</v>
       </c>
@@ -2632,7 +2628,7 @@
       <c r="O9" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="P9" s="45" t="n">
+      <c r="P9" s="44" t="n">
         <f aca="false">SUM(M14:M16)+SUM(M20:M21)</f>
         <v>26633.8</v>
       </c>
@@ -2655,7 +2651,7 @@
       <c r="D10" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F10" s="39" t="n">
@@ -2666,14 +2662,14 @@
       <c r="H10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="47" t="n">
+      <c r="I10" s="46" t="n">
         <f aca="false">(I8+I9)/I6</f>
-        <v>0.18380625</v>
+        <v>0.181235294117647</v>
       </c>
       <c r="K10" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="46" t="s">
+      <c r="L10" s="45" t="s">
         <v>70</v>
       </c>
       <c r="M10" s="39" t="n">
@@ -2683,31 +2679,31 @@
       <c r="O10" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="P10" s="47" t="n">
+      <c r="P10" s="46" t="n">
         <f aca="false">(P8+P9)/P6</f>
         <v>0.247341239716897</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="48"/>
-      <c r="K11" s="49"/>
-      <c r="P11" s="47"/>
-      <c r="R11" s="50"/>
+      <c r="D11" s="47"/>
+      <c r="K11" s="48"/>
+      <c r="P11" s="46"/>
+      <c r="R11" s="49"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
-      <c r="I12" s="52"/>
-      <c r="K12" s="53" t="s">
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="I12" s="51"/>
+      <c r="K12" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="P12" s="54"/>
-      <c r="R12" s="50"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="P12" s="53"/>
+      <c r="R12" s="49"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D13" s="34" t="s">
@@ -2716,24 +2712,24 @@
       <c r="E13" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="52"/>
+      <c r="I13" s="51"/>
       <c r="K13" s="37" t="s">
         <v>47</v>
       </c>
       <c r="L13" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="M13" s="55" t="s">
+      <c r="M13" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="P13" s="54"/>
+      <c r="P13" s="53"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="56"/>
-      <c r="D14" s="57" t="n">
+      <c r="B14" s="43"/>
+      <c r="D14" s="55" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="39" t="n">
@@ -2743,8 +2739,8 @@
         <f aca="false">IF(I$6&lt;=E14, I$5*D14, 0)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="52"/>
-      <c r="K14" s="58" t="n">
+      <c r="I14" s="51"/>
+      <c r="K14" s="56" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="39" t="n">
@@ -2754,10 +2750,10 @@
         <f aca="false">IF(P$6&lt;=L14, P$5*K14, 0)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="54"/>
+      <c r="P14" s="53"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="57" t="n">
+      <c r="D15" s="55" t="n">
         <v>0.15</v>
       </c>
       <c r="E15" s="39" t="n">
@@ -2774,7 +2770,7 @@
         <f aca="false">T9-T8</f>
         <v>24329.16</v>
       </c>
-      <c r="K15" s="58" t="n">
+      <c r="K15" s="56" t="n">
         <v>0.15</v>
       </c>
       <c r="L15" s="39" t="n">
@@ -2787,15 +2783,15 @@
       <c r="O15" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="P15" s="59" t="n">
+      <c r="P15" s="57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="60" t="n">
+      <c r="D16" s="58" t="n">
         <v>0.2</v>
       </c>
-      <c r="E16" s="46" t="s">
+      <c r="E16" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F16" s="21" t="n">
@@ -2807,12 +2803,12 @@
       </c>
       <c r="I16" s="41" t="n">
         <f aca="false">I6+I15</f>
-        <v>184329.16</v>
-      </c>
-      <c r="K16" s="61" t="n">
+        <v>177329.16</v>
+      </c>
+      <c r="K16" s="59" t="n">
         <v>0.2</v>
       </c>
-      <c r="L16" s="46" t="s">
+      <c r="L16" s="45" t="s">
         <v>70</v>
       </c>
       <c r="M16" s="21" t="n">
@@ -2822,13 +2818,13 @@
       <c r="O16" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="P16" s="59" t="n">
+      <c r="P16" s="57" t="n">
         <f aca="false">P6+P15</f>
         <v>494379</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="48"/>
+      <c r="D17" s="47"/>
       <c r="H17" s="0" t="s">
         <v>74</v>
       </c>
@@ -2836,37 +2832,37 @@
         <f aca="false">MIN(B3,MAX(0,B5*(I16-B4)))</f>
         <v>0</v>
       </c>
-      <c r="K17" s="49"/>
+      <c r="K17" s="48"/>
       <c r="O17" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="P17" s="59" t="n">
+      <c r="P17" s="57" t="n">
         <f aca="false">MIN($B3,MAX(0,$B5*(P16-$B4)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="51" t="s">
+      <c r="D18" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
       <c r="H18" s="40" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="41" t="n">
         <f aca="false">I16-B3+I17-I5</f>
-        <v>110729.16</v>
-      </c>
-      <c r="K18" s="53" t="s">
+        <v>103729.16</v>
+      </c>
+      <c r="K18" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
       <c r="O18" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="P18" s="59" t="n">
+      <c r="P18" s="57" t="n">
         <f aca="false">P16+P17-($B3*$B$7)-P5</f>
         <v>285306.32</v>
       </c>
@@ -2878,15 +2874,15 @@
       <c r="E19" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F19" s="54" t="s">
         <v>49</v>
       </c>
       <c r="H19" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="I19" s="45" t="n">
+      <c r="I19" s="44" t="n">
         <f aca="false">F25+F26</f>
-        <v>28789.5816</v>
+        <v>26969.5816</v>
       </c>
       <c r="K19" s="37" t="s">
         <v>47</v>
@@ -2894,19 +2890,19 @@
       <c r="L19" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="M19" s="55" t="s">
+      <c r="M19" s="54" t="s">
         <v>49</v>
       </c>
       <c r="O19" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="P19" s="62" t="n">
+      <c r="P19" s="60" t="n">
         <f aca="false">M25+M26</f>
         <v>75763.7696</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D20" s="63" t="n">
+      <c r="D20" s="61" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="39" t="n">
@@ -2923,7 +2919,7 @@
         <f aca="false">I9</f>
         <v>0</v>
       </c>
-      <c r="K20" s="64" t="n">
+      <c r="K20" s="62" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="39" t="n">
@@ -2942,10 +2938,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="63" t="n">
+      <c r="D21" s="61" t="n">
         <v>0.038</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F21" s="21" t="n">
@@ -2955,14 +2951,14 @@
       <c r="H21" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="47" t="n">
+      <c r="I21" s="46" t="n">
         <f aca="false">(I19+I20)/I16</f>
-        <v>0.156185714729021</v>
-      </c>
-      <c r="K21" s="64" t="n">
+        <v>0.152087685973362</v>
+      </c>
+      <c r="K21" s="62" t="n">
         <v>0.038</v>
       </c>
-      <c r="L21" s="46" t="s">
+      <c r="L21" s="45" t="s">
         <v>70</v>
       </c>
       <c r="M21" s="21" t="n">
@@ -2972,21 +2968,21 @@
       <c r="O21" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="P21" s="47" t="n">
+      <c r="P21" s="46" t="n">
         <f aca="false">(P19+P20)/P16</f>
         <v>0.207123622969422</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="48"/>
+      <c r="D22" s="47"/>
       <c r="H22" s="40" t="s">
         <v>78</v>
       </c>
       <c r="I22" s="41" t="n">
         <f aca="false">IF(I8&gt;I19,((I8+I9)-(I19+I20))/D25,0)</f>
-        <v>2382.37846153846</v>
-      </c>
-      <c r="K22" s="49"/>
+        <v>2920.83999999999</v>
+      </c>
+      <c r="K22" s="48"/>
       <c r="O22" s="40" t="s">
         <v>78</v>
       </c>
@@ -2996,18 +2992,18 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="I23" s="52"/>
-      <c r="K23" s="53" t="s">
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="I23" s="51"/>
+      <c r="K23" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="L23" s="53"/>
-      <c r="M23" s="53"/>
-      <c r="P23" s="54"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="P23" s="53"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="34" t="s">
@@ -3016,20 +3012,20 @@
       <c r="E24" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F24" s="55" t="s">
+      <c r="F24" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="I24" s="52"/>
+      <c r="I24" s="51"/>
       <c r="K24" s="37" t="s">
         <v>47</v>
       </c>
       <c r="L24" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="M24" s="55" t="s">
+      <c r="M24" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="P24" s="54"/>
+      <c r="P24" s="53"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="38" t="s">
@@ -3040,12 +3036,12 @@
       </c>
       <c r="F25" s="21" t="n">
         <f aca="false">MIN((MIN(I18,E25)*D25),((I7-I5)*D25+I9))</f>
-        <v>28789.5816</v>
-      </c>
-      <c r="H25" s="65" t="s">
+        <v>26969.5816</v>
+      </c>
+      <c r="H25" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="I25" s="65"/>
+      <c r="I25" s="63"/>
       <c r="K25" s="42" t="s">
         <v>79</v>
       </c>
@@ -3056,44 +3052,44 @@
         <f aca="false">MIN(P18,L25)*K25</f>
         <v>53586</v>
       </c>
-      <c r="O25" s="66" t="s">
+      <c r="O25" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="P25" s="66"/>
+      <c r="P25" s="64"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="67" t="s">
+      <c r="D26" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="68" t="s">
+      <c r="E26" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="69" t="n">
+      <c r="F26" s="67" t="n">
         <f aca="false">MIN(IF(I18&gt;E25,(I18-E25)*D26, 0),IF((I5-I18)&gt;E25,(I5*D26),0))</f>
         <v>0</v>
       </c>
-      <c r="G26" s="70"/>
-      <c r="H26" s="71" t="n">
+      <c r="G26" s="68"/>
+      <c r="H26" s="69" t="n">
         <f aca="false">I22/Schedule!A1</f>
-        <v>264.708717948717</v>
-      </c>
-      <c r="I26" s="71"/>
-      <c r="K26" s="72" t="s">
+        <v>324.537777777777</v>
+      </c>
+      <c r="I26" s="69"/>
+      <c r="K26" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="L26" s="73" t="s">
+      <c r="L26" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="M26" s="69" t="n">
+      <c r="M26" s="67" t="n">
         <f aca="false">IF(P18&gt;L25,(P18-L25)*K26, 0)</f>
         <v>22177.7696</v>
       </c>
-      <c r="N26" s="74"/>
-      <c r="O26" s="75" t="n">
+      <c r="N26" s="72"/>
+      <c r="O26" s="73" t="n">
         <f aca="false">P22/Schedule!A1</f>
         <v>8496.89963675214</v>
       </c>
-      <c r="P26" s="75"/>
+      <c r="P26" s="73"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D28" s="31" t="s">
@@ -3346,7 +3342,7 @@
       <c r="H35" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="I35" s="45" t="n">
+      <c r="I35" s="44" t="n">
         <f aca="false">SUM(F40:F42)+SUM(F46:F47)</f>
         <v>12220.8145096154</v>
       </c>
@@ -3364,7 +3360,7 @@
       <c r="O35" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="P35" s="45" t="n">
+      <c r="P35" s="44" t="n">
         <f aca="false">SUM(M40:M42)+SUM(M46:M47)</f>
         <v>7175.47017899291</v>
       </c>
@@ -3373,7 +3369,7 @@
       <c r="D36" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="46" t="s">
+      <c r="E36" s="45" t="s">
         <v>70</v>
       </c>
       <c r="F36" s="39" t="n">
@@ -3383,14 +3379,14 @@
       <c r="H36" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="I36" s="47" t="n">
+      <c r="I36" s="46" t="n">
         <f aca="false">(I34+I35)/I32</f>
         <v>0.205198184306893</v>
       </c>
       <c r="K36" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="46" t="s">
+      <c r="L36" s="45" t="s">
         <v>70</v>
       </c>
       <c r="M36" s="39" t="n">
@@ -3400,30 +3396,30 @@
       <c r="O36" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="P36" s="47" t="n">
+      <c r="P36" s="46" t="n">
         <f aca="false">(P34+P35)/P32</f>
         <v>0.188280040468459</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="49"/>
-      <c r="I37" s="47"/>
-      <c r="K37" s="49"/>
-      <c r="P37" s="47"/>
+      <c r="D37" s="48"/>
+      <c r="I37" s="46"/>
+      <c r="K37" s="48"/>
+      <c r="P37" s="46"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="53" t="s">
+      <c r="D38" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="I38" s="54"/>
-      <c r="K38" s="53" t="s">
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="I38" s="53"/>
+      <c r="K38" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="P38" s="54"/>
+      <c r="L38" s="52"/>
+      <c r="M38" s="52"/>
+      <c r="P38" s="53"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D39" s="37" t="s">
@@ -3432,23 +3428,23 @@
       <c r="E39" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F39" s="55" t="s">
+      <c r="F39" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="I39" s="54"/>
+      <c r="I39" s="53"/>
       <c r="K39" s="37" t="s">
         <v>47</v>
       </c>
       <c r="L39" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="M39" s="55" t="s">
+      <c r="M39" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="P39" s="54"/>
+      <c r="P39" s="53"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="58" t="n">
+      <c r="D40" s="56" t="n">
         <v>0</v>
       </c>
       <c r="E40" s="39" t="n">
@@ -3459,8 +3455,8 @@
         <f aca="false">IF(I$32&lt;=E40, I$32*D40, 0)</f>
         <v>0</v>
       </c>
-      <c r="I40" s="54"/>
-      <c r="K40" s="58" t="n">
+      <c r="I40" s="53"/>
+      <c r="K40" s="56" t="n">
         <v>0</v>
       </c>
       <c r="L40" s="39" t="n">
@@ -3471,10 +3467,10 @@
         <f aca="false">IF(P$32&lt;=L40, P$32*K40, 0)</f>
         <v>0</v>
       </c>
-      <c r="P40" s="54"/>
+      <c r="P40" s="53"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="58" t="n">
+      <c r="D41" s="56" t="n">
         <v>0.15</v>
       </c>
       <c r="E41" s="39" t="n">
@@ -3488,10 +3484,10 @@
       <c r="H41" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="59" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" s="58" t="n">
+      <c r="I41" s="57" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" s="56" t="n">
         <v>0.15</v>
       </c>
       <c r="L41" s="39" t="n">
@@ -3505,15 +3501,15 @@
       <c r="O41" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="P41" s="59" t="n">
+      <c r="P41" s="57" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="61" t="n">
+      <c r="D42" s="59" t="n">
         <v>0.2</v>
       </c>
-      <c r="E42" s="76" t="s">
+      <c r="E42" s="74" t="s">
         <v>70</v>
       </c>
       <c r="F42" s="21" t="n">
@@ -3523,14 +3519,14 @@
       <c r="H42" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="I42" s="59" t="n">
+      <c r="I42" s="57" t="n">
         <f aca="false">I32+I41</f>
         <v>331688.096730769</v>
       </c>
-      <c r="K42" s="61" t="n">
+      <c r="K42" s="59" t="n">
         <v>0.2</v>
       </c>
-      <c r="L42" s="46" t="s">
+      <c r="L42" s="45" t="s">
         <v>70</v>
       </c>
       <c r="M42" s="21" t="n">
@@ -3540,51 +3536,51 @@
       <c r="O42" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="P42" s="59" t="n">
+      <c r="P42" s="57" t="n">
         <f aca="false">P32+P41</f>
         <v>254765.467859953</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="49"/>
+      <c r="D43" s="48"/>
       <c r="H43" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="I43" s="59" t="n">
+      <c r="I43" s="57" t="n">
         <f aca="false">MIN($B3,MAX(0,$B5*(I42-$B4)))</f>
         <v>0</v>
       </c>
-      <c r="K43" s="49"/>
+      <c r="K43" s="48"/>
       <c r="O43" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="P43" s="59" t="n">
+      <c r="P43" s="57" t="n">
         <f aca="false">MIN($B29,MAX(0,$B31*(P42-$B30)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="53" t="s">
+      <c r="D44" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
       <c r="H44" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="I44" s="59" t="n">
+      <c r="I44" s="57" t="n">
         <f aca="false">I42+I43-($B3*$B$7^2)-I31</f>
         <v>171936.534816</v>
       </c>
-      <c r="K44" s="53" t="s">
+      <c r="K44" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="L44" s="53"/>
-      <c r="M44" s="53"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
       <c r="O44" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="P44" s="59" t="n">
+      <c r="P44" s="57" t="n">
         <f aca="false">P42+P43-($B3*$B$7^3)-P31</f>
         <v>126199.387555741</v>
       </c>
@@ -3596,13 +3592,13 @@
       <c r="E45" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="55" t="s">
+      <c r="F45" s="54" t="s">
         <v>49</v>
       </c>
       <c r="H45" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="I45" s="62" t="n">
+      <c r="I45" s="60" t="n">
         <f aca="false">F51+F52</f>
         <v>44703.49905216</v>
       </c>
@@ -3612,19 +3608,19 @@
       <c r="L45" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="M45" s="55" t="s">
+      <c r="M45" s="54" t="s">
         <v>49</v>
       </c>
       <c r="O45" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="P45" s="62" t="n">
+      <c r="P45" s="60" t="n">
         <f aca="false">M51+M52</f>
         <v>32811.8407644926</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="64" t="n">
+      <c r="D46" s="62" t="n">
         <v>0</v>
       </c>
       <c r="E46" s="39" t="n">
@@ -3641,7 +3637,7 @@
         <f aca="false">I35</f>
         <v>12220.8145096154</v>
       </c>
-      <c r="K46" s="64" t="n">
+      <c r="K46" s="62" t="n">
         <v>0</v>
       </c>
       <c r="L46" s="39" t="n">
@@ -3660,10 +3656,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="64" t="n">
+      <c r="D47" s="62" t="n">
         <v>0.038</v>
       </c>
-      <c r="E47" s="76" t="s">
+      <c r="E47" s="74" t="s">
         <v>70</v>
       </c>
       <c r="F47" s="21" t="n">
@@ -3673,14 +3669,14 @@
       <c r="H47" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="I47" s="47" t="n">
+      <c r="I47" s="46" t="n">
         <f aca="false">I45/I42</f>
         <v>0.134775710954879</v>
       </c>
-      <c r="K47" s="64" t="n">
+      <c r="K47" s="62" t="n">
         <v>0.038</v>
       </c>
-      <c r="L47" s="46" t="s">
+      <c r="L47" s="45" t="s">
         <v>70</v>
       </c>
       <c r="M47" s="21" t="n">
@@ -3690,13 +3686,13 @@
       <c r="O47" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="P47" s="47" t="n">
+      <c r="P47" s="46" t="n">
         <f aca="false">P45/P42</f>
         <v>0.128792340029888</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="49"/>
+      <c r="D48" s="48"/>
       <c r="H48" s="40" t="s">
         <v>78</v>
       </c>
@@ -3704,7 +3700,7 @@
         <f aca="false">IF(I34&gt;I45,((I34+I35)-(I45+I46))/D51,0)</f>
         <v>42836.4678599527</v>
       </c>
-      <c r="K48" s="49"/>
+      <c r="K48" s="48"/>
       <c r="O48" s="40" t="s">
         <v>78</v>
       </c>
@@ -3714,18 +3710,18 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="53" t="s">
+      <c r="D49" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="I49" s="54"/>
-      <c r="K49" s="53" t="s">
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="I49" s="53"/>
+      <c r="K49" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="L49" s="53"/>
-      <c r="M49" s="53"/>
-      <c r="P49" s="54"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="P49" s="53"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D50" s="37" t="s">
@@ -3734,20 +3730,20 @@
       <c r="E50" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F50" s="55" t="s">
+      <c r="F50" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="I50" s="54"/>
+      <c r="I50" s="53"/>
       <c r="K50" s="37" t="s">
         <v>47</v>
       </c>
       <c r="L50" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="M50" s="55" t="s">
+      <c r="M50" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="P50" s="54"/>
+      <c r="P50" s="53"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D51" s="42" t="s">
@@ -3761,10 +3757,10 @@
         <f aca="false">MIN(I44,E51)*D51</f>
         <v>44703.49905216</v>
       </c>
-      <c r="H51" s="66" t="s">
+      <c r="H51" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="I51" s="66"/>
+      <c r="I51" s="64"/>
       <c r="K51" s="42" t="s">
         <v>79</v>
       </c>
@@ -3776,44 +3772,44 @@
         <f aca="false">MIN(P44,L51)*K51</f>
         <v>32811.8407644926</v>
       </c>
-      <c r="O51" s="66" t="s">
+      <c r="O51" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="P51" s="66"/>
+      <c r="P51" s="64"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="72" t="s">
+      <c r="D52" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="E52" s="73" t="s">
+      <c r="E52" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="F52" s="69" t="n">
+      <c r="F52" s="67" t="n">
         <f aca="false">IF(I44&gt;E51,(I44-E51)*D52, 0)</f>
         <v>0</v>
       </c>
-      <c r="G52" s="74"/>
-      <c r="H52" s="75" t="n">
+      <c r="G52" s="72"/>
+      <c r="H52" s="73" t="n">
         <f aca="false">I48/Schedule!$A$1</f>
         <v>4759.60753999475</v>
       </c>
-      <c r="I52" s="75"/>
-      <c r="K52" s="72" t="s">
+      <c r="I52" s="73"/>
+      <c r="K52" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="L52" s="73" t="s">
+      <c r="L52" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="M52" s="69" t="n">
+      <c r="M52" s="67" t="n">
         <f aca="false">IF(P44&gt;L51,(P44-L51)*K52, 0)</f>
         <v>0</v>
       </c>
-      <c r="N52" s="74"/>
-      <c r="O52" s="75" t="n">
+      <c r="N52" s="72"/>
+      <c r="O52" s="73" t="n">
         <f aca="false">P48/Schedule!$A$1</f>
         <v>3410.23147656082</v>
       </c>
-      <c r="P52" s="75"/>
+      <c r="P52" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -3892,175 +3888,175 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="79" t="n">
+      <c r="A1" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="77" t="n">
         <f aca="false">N1*Q1</f>
         <v>0.8436</v>
       </c>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79" t="n">
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77" t="n">
         <v>9.25</v>
       </c>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="80" t="n">
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="78" t="n">
         <f aca="false">0.0912</f>
         <v>0.0912</v>
       </c>
-      <c r="R1" s="80"/>
+      <c r="R1" s="78"/>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="82" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
+      <c r="L2" s="80"/>
+      <c r="M2" s="80"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="83" t="s">
+      <c r="H3" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="83" t="s">
+      <c r="I3" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="84"/>
-      <c r="K3" s="83" t="s">
+      <c r="J3" s="82"/>
+      <c r="K3" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="83" t="s">
+      <c r="L3" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="M3" s="83" t="s">
+      <c r="M3" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="N3" s="83" t="s">
+      <c r="N3" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="83" t="s">
+      <c r="O3" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="83" t="s">
+      <c r="P3" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="Q3" s="85" t="s">
+      <c r="Q3" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="R3" s="85" t="s">
+      <c r="R3" s="83" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="86" t="n">
+      <c r="A4" s="84" t="n">
         <v>42457</v>
       </c>
-      <c r="B4" s="87" t="n">
+      <c r="B4" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C4" s="88" t="n">
+      <c r="C4" s="86" t="n">
         <v>30000</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="90" t="n">
+      <c r="E4" s="88" t="n">
         <f aca="false">MAX(0,MIN(48*0.75,DATEDIF(A4,C18,"M")-12))</f>
         <v>36</v>
       </c>
-      <c r="F4" s="91" t="n">
+      <c r="F4" s="89" t="n">
         <f aca="false">0.25*C4*IF(DATEDIF(A4,$C$18,"Y")&gt;=1, 1, 0) + 0.75*C4*IF(DATEDIF(A4,$C$18,"Y")&gt;=1, MIN(36,E4)/36, 0)</f>
         <v>30000</v>
       </c>
-      <c r="G4" s="88" t="n">
+      <c r="G4" s="86" t="n">
         <v>30000</v>
       </c>
-      <c r="H4" s="92" t="n">
+      <c r="H4" s="90" t="n">
         <f aca="false">IF(F4=C4, 0, IF(DATEDIF(A4,$C$18,"Y")&gt;=1, C4*0.75/48, 0))</f>
         <v>0</v>
       </c>
-      <c r="I4" s="86" t="n">
+      <c r="I4" s="84" t="n">
         <f aca="false">DATE(YEAR(A4)+1, MONTH(A4)+(0.75*48), DAY(A4))</f>
         <v>43918</v>
       </c>
-      <c r="J4" s="93"/>
-      <c r="K4" s="86" t="n">
+      <c r="J4" s="91"/>
+      <c r="K4" s="84" t="n">
         <v>42457</v>
       </c>
-      <c r="L4" s="86" t="n">
+      <c r="L4" s="84" t="n">
         <v>44001</v>
       </c>
-      <c r="M4" s="87" t="n">
+      <c r="M4" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="N4" s="88" t="n">
+      <c r="N4" s="86" t="n">
         <v>30000</v>
       </c>
-      <c r="O4" s="94" t="n">
+      <c r="O4" s="92" t="n">
         <f aca="false">N4*M4</f>
         <v>33</v>
       </c>
-      <c r="P4" s="95" t="n">
+      <c r="P4" s="93" t="n">
         <f aca="false">N4*K$1</f>
         <v>25308</v>
       </c>
-      <c r="Q4" s="86" t="n">
+      <c r="Q4" s="84" t="n">
         <f aca="false">MAX(DATE(YEAR(L4)+1,MONTH(L4),DAY(L4)),DATE(YEAR(K4)+2,MONTH(K4),DAY(K4)))</f>
         <v>44366</v>
       </c>
-      <c r="R4" s="96" t="n">
+      <c r="R4" s="94" t="n">
         <f aca="false">IF($C$18&gt;Q4, P4*0.15, P4*0.35)</f>
         <v>3796.2</v>
       </c>
-      <c r="T4" s="97" t="n">
+      <c r="T4" s="95" t="n">
         <v>0.000276</v>
       </c>
       <c r="U4" s="20" t="n">
@@ -4069,67 +4065,67 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86" t="n">
+      <c r="A5" s="84" t="n">
         <v>43447</v>
       </c>
-      <c r="B5" s="87" t="n">
+      <c r="B5" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C5" s="88" t="n">
+      <c r="C5" s="86" t="n">
         <v>123519</v>
       </c>
-      <c r="D5" s="89" t="s">
+      <c r="D5" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="90" t="n">
+      <c r="E5" s="88" t="n">
         <f aca="false">MAX(0,MIN(36,DATEDIF(A5,C18,"M")))</f>
         <v>36</v>
       </c>
-      <c r="F5" s="91" t="n">
+      <c r="F5" s="89" t="n">
         <f aca="false">C5*0.35+(C5*0.65)*MIN(36,E5)/36</f>
         <v>123519</v>
       </c>
-      <c r="G5" s="98" t="n">
+      <c r="G5" s="96" t="n">
         <v>83375</v>
       </c>
-      <c r="H5" s="92" t="n">
+      <c r="H5" s="90" t="n">
         <f aca="false">IF(F5=C5, 0, C5*0.65/36)</f>
         <v>0</v>
       </c>
-      <c r="I5" s="86" t="n">
+      <c r="I5" s="84" t="n">
         <f aca="false">DATE(YEAR(A5), MONTH(A5)+36, DAY(A5))</f>
         <v>44543</v>
       </c>
-      <c r="J5" s="99"/>
-      <c r="K5" s="86" t="n">
+      <c r="J5" s="97"/>
+      <c r="K5" s="84" t="n">
         <v>43447</v>
       </c>
-      <c r="L5" s="86" t="n">
+      <c r="L5" s="84" t="n">
         <v>44001</v>
       </c>
-      <c r="M5" s="87" t="n">
+      <c r="M5" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="N5" s="98" t="n">
+      <c r="N5" s="96" t="n">
         <v>83375</v>
       </c>
-      <c r="O5" s="94" t="n">
+      <c r="O5" s="92" t="n">
         <f aca="false">M5*N5</f>
         <v>91.7125</v>
       </c>
-      <c r="P5" s="95" t="n">
+      <c r="P5" s="93" t="n">
         <f aca="false">N5*K$1</f>
         <v>70335.15</v>
       </c>
-      <c r="Q5" s="86" t="n">
+      <c r="Q5" s="84" t="n">
         <f aca="false">MAX(DATE(YEAR(L5)+1,MONTH(L5),DAY(L5)),DATE(YEAR(K5)+2,MONTH(K5),DAY(K5)))</f>
         <v>44366</v>
       </c>
-      <c r="R5" s="96" t="n">
+      <c r="R5" s="94" t="n">
         <f aca="false">IF($C$18&gt;Q5, P5*0.15, P5*0.35)</f>
         <v>10550.2725</v>
       </c>
-      <c r="T5" s="97" t="n">
+      <c r="T5" s="95" t="n">
         <v>0.000766</v>
       </c>
       <c r="U5" s="20" t="n">
@@ -4138,67 +4134,67 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="86" t="n">
+      <c r="A6" s="84" t="n">
         <v>43602</v>
       </c>
-      <c r="B6" s="87" t="n">
+      <c r="B6" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C6" s="88" t="n">
+      <c r="C6" s="86" t="n">
         <v>38380</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="90" t="n">
+      <c r="E6" s="88" t="n">
         <f aca="false">MAX(0,MIN(48*0.75,DATEDIF(A6,C$18,"M")-12))</f>
         <v>23</v>
       </c>
-      <c r="F6" s="91" t="n">
+      <c r="F6" s="89" t="n">
         <f aca="false">0.25*C6*IF(DATEDIF(A6,$C$18,"Y")&gt;=1, 1, 0) + 0.75*C6*IF(DATEDIF(A6,$C$18,"Y")&gt;=1, MIN(36,E6)/36, 0)</f>
         <v>27985.4166666667</v>
       </c>
-      <c r="G6" s="98" t="n">
+      <c r="G6" s="96" t="n">
         <v>10394</v>
       </c>
-      <c r="H6" s="92" t="n">
+      <c r="H6" s="90" t="n">
         <f aca="false">IF(F6=C6, 0, IF(DATEDIF(A6,$C$18,"Y")&gt;=1, C6/48, 0))</f>
         <v>799.583333333333</v>
       </c>
-      <c r="I6" s="86" t="n">
+      <c r="I6" s="84" t="n">
         <f aca="false">DATE(YEAR(A6)+1, MONTH(A6)+(48*0.75), DAY(A6))</f>
         <v>45063</v>
       </c>
-      <c r="J6" s="99"/>
-      <c r="K6" s="100" t="n">
+      <c r="J6" s="97"/>
+      <c r="K6" s="98" t="n">
         <v>43602</v>
       </c>
-      <c r="L6" s="100" t="n">
+      <c r="L6" s="98" t="n">
         <v>44001</v>
       </c>
-      <c r="M6" s="101" t="n">
+      <c r="M6" s="99" t="n">
         <v>0.0011</v>
       </c>
-      <c r="N6" s="102" t="n">
+      <c r="N6" s="100" t="n">
         <v>10394</v>
       </c>
-      <c r="O6" s="103" t="n">
+      <c r="O6" s="101" t="n">
         <f aca="false">M6*N6</f>
         <v>11.4334</v>
       </c>
-      <c r="P6" s="104" t="n">
+      <c r="P6" s="102" t="n">
         <f aca="false">N6*K$1</f>
         <v>8768.3784</v>
       </c>
-      <c r="Q6" s="100" t="n">
+      <c r="Q6" s="98" t="n">
         <f aca="false">MAX(DATE(YEAR(L6)+1,MONTH(L6),DAY(L6)),DATE(YEAR(K6)+2,MONTH(K6),DAY(K6)))</f>
         <v>44366</v>
       </c>
-      <c r="R6" s="105" t="n">
+      <c r="R6" s="103" t="n">
         <f aca="false">IF($C$18&gt;Q6, P6*0.15, P6*0.35)</f>
         <v>1315.25676</v>
       </c>
-      <c r="T6" s="97" t="n">
+      <c r="T6" s="95" t="n">
         <v>9.6E-005</v>
       </c>
       <c r="U6" s="20" t="n">
@@ -4207,394 +4203,394 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="86" t="n">
+      <c r="A7" s="84" t="n">
         <v>43769</v>
       </c>
-      <c r="B7" s="87" t="n">
+      <c r="B7" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C7" s="88" t="n">
+      <c r="C7" s="86" t="n">
         <v>138965</v>
       </c>
-      <c r="D7" s="89" t="s">
+      <c r="D7" s="87" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="90" t="n">
+      <c r="E7" s="88" t="n">
         <f aca="false">MAX(0,MIN(48*0.75,DATEDIF(A7,C$18,"M")-12))</f>
         <v>17</v>
       </c>
-      <c r="F7" s="91" t="n">
+      <c r="F7" s="89" t="n">
         <f aca="false">0.25*C7*IF(DATEDIF(A7,$C$18,"Y")&gt;=1, 1, 0) + 0.75*C7*IF(DATEDIF(A7,$C$18,"Y")&gt;=1, MIN(36,E7)/36, 0)</f>
         <v>83958.0208333333</v>
       </c>
-      <c r="G7" s="88" t="n">
+      <c r="G7" s="86" t="n">
         <v>32400</v>
       </c>
-      <c r="H7" s="92" t="n">
+      <c r="H7" s="90" t="n">
         <f aca="false">IF(F7=C7, 0, IF(DATEDIF(A7,$C$18,"Y")&gt;=1, C7/48, 0))</f>
         <v>2895.10416666667</v>
       </c>
-      <c r="I7" s="86" t="n">
+      <c r="I7" s="84" t="n">
         <f aca="false">DATE(YEAR(A7)+1, MONTH(A7)+(48*0.75), DAY(A7))</f>
         <v>45230</v>
       </c>
-      <c r="J7" s="93"/>
-      <c r="Q7" s="106"/>
+      <c r="J7" s="91"/>
+      <c r="Q7" s="104"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="86" t="n">
+      <c r="A8" s="84" t="n">
         <v>44263</v>
       </c>
-      <c r="B8" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="88" t="n">
+      <c r="B8" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="86" t="n">
         <v>330000</v>
       </c>
-      <c r="D8" s="107" t="s">
+      <c r="D8" s="105" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="90" t="n">
+      <c r="E8" s="88" t="n">
         <f aca="false">MAX(0,MIN(48*0.75,DATEDIF(A8,C$18,"M")-12))</f>
         <v>1</v>
       </c>
-      <c r="F8" s="91" t="n">
+      <c r="F8" s="89" t="n">
         <f aca="false">0.5*C8*IF($C$18 &gt;= DATE(2022,1,1), 1, 0) + 0.5*C8*IF(DATEDIF(A8,$C$18,"Y")&gt;=1, MIN(36,E8)/36, 0)</f>
         <v>169583.333333333</v>
       </c>
-      <c r="G8" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="92" t="n">
+      <c r="G8" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="90" t="n">
         <f aca="false">IF(F8=C8, 0, IF($C$18 &gt;= L9, C8*0.75/36, 0))</f>
         <v>6875</v>
       </c>
-      <c r="I8" s="86" t="n">
+      <c r="I8" s="84" t="n">
         <f aca="false">DATE(YEAR(A8), MONTH(A8)+36, DAY(A8))</f>
         <v>45359</v>
       </c>
-      <c r="J8" s="93"/>
-      <c r="K8" s="86" t="n">
+      <c r="J8" s="91"/>
+      <c r="K8" s="84" t="n">
         <v>43769</v>
       </c>
-      <c r="L8" s="108" t="n">
+      <c r="L8" s="106" t="n">
         <v>44324</v>
       </c>
-      <c r="M8" s="87" t="n">
+      <c r="M8" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="N8" s="88" t="n">
+      <c r="N8" s="86" t="n">
         <v>32400</v>
       </c>
-      <c r="O8" s="94" t="n">
+      <c r="O8" s="92" t="n">
         <f aca="false">M8*N8</f>
         <v>35.64</v>
       </c>
-      <c r="P8" s="95" t="n">
+      <c r="P8" s="93" t="n">
         <f aca="false">N8*$K$1</f>
         <v>27332.64</v>
       </c>
-      <c r="Q8" s="106" t="n">
+      <c r="Q8" s="104" t="n">
         <f aca="false">MAX(DATE(YEAR(L8)+1,MONTH(L8),DAY(L8)),DATE(YEAR(K8)+2,MONTH(K8),DAY(K8)))</f>
         <v>44689</v>
       </c>
-      <c r="R8" s="96" t="n">
+      <c r="R8" s="94" t="n">
         <f aca="false">IF($C$18&gt;Q8, P8*0.15, P8*0.35)</f>
         <v>9566.424</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="109"/>
-      <c r="K9" s="86" t="n">
+      <c r="A9" s="88"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="107"/>
+      <c r="K9" s="84" t="n">
         <v>44263</v>
       </c>
-      <c r="L9" s="108" t="n">
+      <c r="L9" s="106" t="n">
         <v>44642</v>
       </c>
-      <c r="M9" s="87" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="88" t="n">
+      <c r="M9" s="85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="86" t="n">
         <v>165000</v>
       </c>
-      <c r="O9" s="94" t="n">
+      <c r="O9" s="92" t="n">
         <f aca="false">M9*N9</f>
         <v>0</v>
       </c>
-      <c r="P9" s="95" t="n">
+      <c r="P9" s="93" t="n">
         <f aca="false">N9*$K$1</f>
         <v>139194</v>
       </c>
-      <c r="Q9" s="106" t="n">
+      <c r="Q9" s="104" t="n">
         <f aca="false">MAX(DATE(YEAR(L9)+1,MONTH(L9),DAY(L9)),DATE(YEAR(K9)+2,MONTH(K9),DAY(K9)))</f>
         <v>45007</v>
       </c>
-      <c r="R9" s="96" t="n">
+      <c r="R9" s="94" t="n">
         <f aca="false">IF($C$18&gt;Q9, P9*0.15, P9*0.35)</f>
         <v>48717.9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="110"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="109"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="108"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="94"/>
-      <c r="P10" s="95"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="96"/>
+      <c r="A10" s="108"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="106"/>
+      <c r="M10" s="85"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="92"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="84"/>
+      <c r="R10" s="94"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="109"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="94"/>
-      <c r="P11" s="95"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
+      <c r="A11" s="86"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="107"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="88"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="92"/>
+      <c r="P11" s="93"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="88"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="111"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="109"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="95"/>
-      <c r="O12" s="94"/>
-      <c r="P12" s="90"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="90"/>
+      <c r="A12" s="109"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="88"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="93"/>
+      <c r="O12" s="92"/>
+      <c r="P12" s="88"/>
+      <c r="Q12" s="88"/>
+      <c r="R12" s="88"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="112"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="90"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="114"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="90"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="95"/>
-      <c r="O13" s="94"/>
-      <c r="P13" s="90"/>
-      <c r="Q13" s="90"/>
-      <c r="R13" s="90"/>
+      <c r="A13" s="110"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="88"/>
+      <c r="M13" s="88"/>
+      <c r="N13" s="93"/>
+      <c r="O13" s="92"/>
+      <c r="P13" s="88"/>
+      <c r="Q13" s="88"/>
+      <c r="R13" s="88"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="86"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="109"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="95"/>
-      <c r="O14" s="94"/>
-      <c r="P14" s="90"/>
-      <c r="Q14" s="90"/>
-      <c r="R14" s="90"/>
+      <c r="A14" s="84"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="107"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="93"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="88"/>
+      <c r="Q14" s="88"/>
+      <c r="R14" s="88"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="86"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="109"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="95"/>
-      <c r="O15" s="90"/>
-      <c r="P15" s="90"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
+      <c r="A15" s="84"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="107"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="88"/>
+      <c r="P15" s="88"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="88"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="115" t="str">
+      <c r="A16" s="113" t="str">
         <f aca="false">"Grants: "&amp;COUNT(A4:A7)</f>
         <v>Grants: 4</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="117" t="n">
+      <c r="B16" s="114"/>
+      <c r="C16" s="115" t="n">
         <f aca="false">SUM(C4:C14)</f>
         <v>660864</v>
       </c>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="119" t="n">
+      <c r="D16" s="115"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="117" t="n">
         <f aca="false">SUM(F4:F14)</f>
         <v>435045.770833333</v>
       </c>
-      <c r="G16" s="117" t="n">
+      <c r="G16" s="115" t="n">
         <f aca="false">SUM(G4:G14)</f>
         <v>156169</v>
       </c>
-      <c r="H16" s="120" t="n">
+      <c r="H16" s="118" t="n">
         <f aca="false">SUM(H4:H8)*K1</f>
         <v>8916.588375</v>
       </c>
-      <c r="I16" s="121"/>
-      <c r="J16" s="122"/>
-      <c r="K16" s="123" t="s">
+      <c r="I16" s="119"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="L16" s="123"/>
-      <c r="M16" s="123"/>
-      <c r="N16" s="123"/>
-      <c r="O16" s="123"/>
-      <c r="P16" s="124" t="n">
+      <c r="L16" s="121"/>
+      <c r="M16" s="121"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="122" t="n">
         <f aca="false">SUM(P4:P10)</f>
         <v>270938.1684</v>
       </c>
-      <c r="Q16" s="124"/>
-      <c r="R16" s="124"/>
+      <c r="Q16" s="122"/>
+      <c r="R16" s="122"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="125" t="s">
+      <c r="A17" s="123" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="126"/>
-      <c r="C17" s="127" t="n">
+      <c r="B17" s="124"/>
+      <c r="C17" s="125" t="n">
         <f aca="false">SUM(H4:H14)</f>
         <v>10569.6875</v>
       </c>
-      <c r="D17" s="127"/>
-      <c r="E17" s="128"/>
-      <c r="F17" s="129" t="n">
+      <c r="D17" s="125"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="127" t="n">
         <f aca="false">F16/C16</f>
         <v>0.658298486274534</v>
       </c>
-      <c r="G17" s="129" t="n">
+      <c r="G17" s="127" t="n">
         <f aca="false">G16/F16</f>
         <v>0.358971424319002</v>
       </c>
-      <c r="H17" s="128"/>
-      <c r="I17" s="128"/>
-      <c r="J17" s="130"/>
-      <c r="K17" s="123" t="s">
+      <c r="H17" s="126"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="128"/>
+      <c r="K17" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="L17" s="123"/>
-      <c r="M17" s="123"/>
-      <c r="N17" s="123"/>
-      <c r="O17" s="123"/>
-      <c r="P17" s="131" t="n">
+      <c r="L17" s="121"/>
+      <c r="M17" s="121"/>
+      <c r="N17" s="121"/>
+      <c r="O17" s="121"/>
+      <c r="P17" s="129" t="n">
         <f aca="false">SUM(R4:R10)</f>
         <v>73946.05326</v>
       </c>
-      <c r="Q17" s="131"/>
-      <c r="R17" s="131"/>
+      <c r="Q17" s="129"/>
+      <c r="R17" s="129"/>
     </row>
     <row r="18" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="86"/>
-      <c r="B18" s="85" t="s">
+      <c r="A18" s="84"/>
+      <c r="B18" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="132" t="n">
+      <c r="C18" s="130" t="n">
         <v>44671</v>
       </c>
-      <c r="D18" s="88"/>
-      <c r="E18" s="90"/>
-      <c r="F18" s="90"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="133" t="n">
+      <c r="D18" s="86"/>
+      <c r="E18" s="88"/>
+      <c r="F18" s="88"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="131" t="n">
         <f aca="false">H16*12</f>
         <v>106999.0605</v>
       </c>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="134" t="s">
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="134"/>
-      <c r="M18" s="134"/>
-      <c r="N18" s="134"/>
-      <c r="O18" s="134"/>
-      <c r="P18" s="135" t="n">
+      <c r="L18" s="132"/>
+      <c r="M18" s="132"/>
+      <c r="N18" s="132"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="133" t="n">
         <f aca="false">P16-P17</f>
         <v>196992.11514</v>
       </c>
-      <c r="Q18" s="135"/>
-      <c r="R18" s="135"/>
+      <c r="Q18" s="133"/>
+      <c r="R18" s="133"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="86"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="88"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="90"/>
-      <c r="K19" s="136" t="s">
+      <c r="A19" s="84"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="134" t="s">
         <v>104</v>
       </c>
-      <c r="L19" s="136"/>
-      <c r="M19" s="136"/>
-      <c r="N19" s="136"/>
-      <c r="O19" s="136"/>
-      <c r="P19" s="137" t="n">
+      <c r="L19" s="134"/>
+      <c r="M19" s="134"/>
+      <c r="N19" s="134"/>
+      <c r="O19" s="134"/>
+      <c r="P19" s="135" t="n">
         <f aca="false">(C16-G16)*K1*0.65</f>
         <v>276744.4563</v>
       </c>
-      <c r="Q19" s="137"/>
-      <c r="R19" s="137"/>
+      <c r="Q19" s="135"/>
+      <c r="R19" s="135"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="N23" s="0" t="n">
@@ -4682,7 +4678,7 @@
       <c r="B1" s="21" t="n">
         <v>12550</v>
       </c>
-      <c r="C1" s="138"/>
+      <c r="C1" s="136"/>
       <c r="D1" s="0" t="s">
         <v>58</v>
       </c>
@@ -4690,7 +4686,7 @@
         <f aca="false">B8-B1+E2</f>
         <v>237450</v>
       </c>
-      <c r="F1" s="139"/>
+      <c r="F1" s="137"/>
       <c r="I1" s="7" t="s">
         <v>45</v>
       </c>
@@ -4714,12 +4710,12 @@
       <c r="B2" s="0" t="n">
         <v>73600</v>
       </c>
-      <c r="C2" s="138"/>
+      <c r="C2" s="136"/>
       <c r="D2" s="0" t="s">
         <v>105</v>
       </c>
       <c r="E2" s="21"/>
-      <c r="F2" s="139"/>
+      <c r="F2" s="137"/>
       <c r="I2" s="21" t="n">
         <f aca="false">MAX(0,E1-B18)*A19+MIN(B18-B17,MAX(0,E1-B17))*A18+MIN(B17-B16,MAX(0,E1-B16))*A17+MIN(B16-B15,MAX(0,E1-B15))*A16+MIN(B15-B14,MAX(0,E1-B14))*A15+MIN(B14-B13,MAX(0,E1-B13))*A14+MIN(B13,MAX(0,E1))*A13+MAX(0,IF(E4&gt;E13,(E4-E13)*D14, 0))+MAX(0,IF(E4&gt;B23,MIN((B24-B23),(E3-B23))*A24, 0))+MAX(0,IF(E4&gt;B24,(E3-B24)*A25, 0))</f>
         <v>59074.85</v>
@@ -4752,12 +4748,12 @@
       <c r="B3" s="0" t="n">
         <v>523600</v>
       </c>
-      <c r="C3" s="138"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="0" t="s">
         <v>55</v>
       </c>
       <c r="E3" s="21"/>
-      <c r="F3" s="140"/>
+      <c r="F3" s="138"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -4766,7 +4762,7 @@
       <c r="B4" s="27" t="n">
         <v>0.25</v>
       </c>
-      <c r="C4" s="138"/>
+      <c r="C4" s="136"/>
       <c r="D4" s="0" t="s">
         <v>106</v>
       </c>
@@ -4774,7 +4770,7 @@
         <f aca="false">E1+E3</f>
         <v>237450</v>
       </c>
-      <c r="F4" s="140"/>
+      <c r="F4" s="138"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -4783,14 +4779,14 @@
       <c r="B5" s="11" t="n">
         <v>44378</v>
       </c>
-      <c r="C5" s="138"/>
+      <c r="C5" s="136"/>
       <c r="D5" s="0" t="s">
         <v>72</v>
       </c>
       <c r="E5" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="139"/>
+      <c r="F5" s="137"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -4799,7 +4795,7 @@
       <c r="B6" s="0" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="138"/>
+      <c r="C6" s="136"/>
       <c r="D6" s="0" t="s">
         <v>109</v>
       </c>
@@ -4807,9 +4803,9 @@
         <f aca="false">B8+E2+E3+E5</f>
         <v>250000</v>
       </c>
-      <c r="F6" s="139"/>
-      <c r="I6" s="50"/>
-      <c r="K6" s="50"/>
+      <c r="F6" s="137"/>
+      <c r="I6" s="49"/>
+      <c r="K6" s="49"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -4819,7 +4815,7 @@
         <f aca="false">B5+B6</f>
         <v>44558</v>
       </c>
-      <c r="C7" s="138"/>
+      <c r="C7" s="136"/>
       <c r="D7" s="0" t="s">
         <v>111</v>
       </c>
@@ -4827,17 +4823,17 @@
         <f aca="false">MIN(B2,MAX(0,B4*(E6-B3)))</f>
         <v>0</v>
       </c>
-      <c r="F7" s="139"/>
+      <c r="F7" s="137"/>
       <c r="I7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B8" s="55" t="n">
+      <c r="B8" s="54" t="n">
         <v>250000</v>
       </c>
-      <c r="C8" s="139"/>
+      <c r="C8" s="137"/>
       <c r="D8" s="40" t="s">
         <v>76</v>
       </c>
@@ -4845,7 +4841,7 @@
         <f aca="false">E6-B2+E7</f>
         <v>176400</v>
       </c>
-      <c r="F8" s="139"/>
+      <c r="F8" s="137"/>
       <c r="I8" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4867,7 +4863,7 @@
       <c r="B12" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="141"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="35" t="s">
         <v>47</v>
       </c>
@@ -4877,14 +4873,14 @@
       <c r="F12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="142" t="s">
+      <c r="A13" s="140" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="39" t="n">
         <v>9950</v>
       </c>
-      <c r="C13" s="143"/>
-      <c r="D13" s="144" t="n">
+      <c r="C13" s="141"/>
+      <c r="D13" s="142" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="39" t="n">
@@ -4893,36 +4889,36 @@
       <c r="F13" s="21"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="142" t="s">
+      <c r="A14" s="140" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="39" t="n">
         <v>40525</v>
       </c>
-      <c r="C14" s="143"/>
-      <c r="D14" s="144" t="n">
+      <c r="C14" s="141"/>
+      <c r="D14" s="142" t="n">
         <v>0.038</v>
       </c>
       <c r="F14" s="21"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="142" t="s">
+      <c r="A15" s="140" t="s">
         <v>57</v>
       </c>
       <c r="B15" s="39" t="n">
         <v>86375</v>
       </c>
-      <c r="C15" s="143"/>
+      <c r="C15" s="141"/>
       <c r="F15" s="21"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="142" t="s">
+      <c r="A16" s="140" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="39" t="n">
         <v>164925</v>
       </c>
-      <c r="C16" s="143"/>
+      <c r="C16" s="141"/>
       <c r="D16" s="19" t="s">
         <v>77</v>
       </c>
@@ -4930,13 +4926,13 @@
       <c r="F16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="142" t="s">
+      <c r="A17" s="140" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="39" t="n">
         <v>209425</v>
       </c>
-      <c r="C17" s="143"/>
+      <c r="C17" s="141"/>
       <c r="D17" s="35" t="s">
         <v>47</v>
       </c>
@@ -4944,17 +4940,17 @@
         <v>48</v>
       </c>
       <c r="F17" s="26"/>
-      <c r="G17" s="50"/>
+      <c r="G17" s="49"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="142" t="s">
+      <c r="A18" s="140" t="s">
         <v>66</v>
       </c>
       <c r="B18" s="39" t="n">
         <v>523600</v>
       </c>
-      <c r="C18" s="143"/>
-      <c r="D18" s="142" t="s">
+      <c r="C18" s="141"/>
+      <c r="D18" s="140" t="s">
         <v>79</v>
       </c>
       <c r="E18" s="39" t="n">
@@ -4962,15 +4958,15 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="142" t="s">
+      <c r="A19" s="140" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="145"/>
-      <c r="C19" s="143"/>
-      <c r="D19" s="142" t="s">
+      <c r="B19" s="143"/>
+      <c r="C19" s="141"/>
+      <c r="D19" s="140" t="s">
         <v>81</v>
       </c>
-      <c r="E19" s="145"/>
+      <c r="E19" s="143"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19" t="s">
@@ -4986,34 +4982,34 @@
       <c r="B22" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="43"/>
+      <c r="C22" s="144"/>
       <c r="F22" s="21"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="146" t="n">
+      <c r="A23" s="145" t="n">
         <v>0</v>
       </c>
       <c r="B23" s="39" t="n">
         <v>40400</v>
       </c>
-      <c r="C23" s="50"/>
+      <c r="C23" s="49"/>
       <c r="F23" s="21"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="146" t="n">
+      <c r="A24" s="145" t="n">
         <v>0.15</v>
       </c>
-      <c r="B24" s="145" t="n">
+      <c r="B24" s="143" t="n">
         <v>445850</v>
       </c>
-      <c r="C24" s="50"/>
+      <c r="C24" s="49"/>
       <c r="F24" s="21"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="147" t="n">
+      <c r="A25" s="146" t="n">
         <v>0.2</v>
       </c>
-      <c r="C25" s="50"/>
+      <c r="C25" s="49"/>
       <c r="F25" s="21"/>
     </row>
   </sheetData>
@@ -5046,949 +5042,949 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="148" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="148" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="148" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="149" width="5.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="148" width="18.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="148" width="4.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="148" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="148" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="148" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="148" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="148" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="148" width="5.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="148" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="148" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="148" width="7.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="148" width="9.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="148" width="6.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="148" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="148" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="147" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="147" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="147" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="148" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="147" width="18.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="147" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="147" width="4.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="147" width="13.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="147" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="147" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="147" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="147" width="5.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="147" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="147" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="147" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="147" width="9.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="147" width="6.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="147" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="147" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="77" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="79" t="n">
+      <c r="A1" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="77" t="n">
         <v>2.5</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="85"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="83"/>
       <c r="V1" s="0"/>
       <c r="W1" s="0"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="79" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="82" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="80" t="s">
         <v>83</v>
       </c>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="85"/>
-      <c r="V2" s="85"/>
-      <c r="W2" s="85"/>
-      <c r="X2" s="85"/>
-      <c r="Y2" s="85"/>
-      <c r="Z2" s="85"/>
-      <c r="AA2" s="85"/>
-      <c r="AB2" s="85"/>
-      <c r="AC2" s="85"/>
-      <c r="AD2" s="85"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="83"/>
+      <c r="AB2" s="83"/>
+      <c r="AC2" s="83"/>
+      <c r="AD2" s="83"/>
     </row>
     <row r="3" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="83" t="s">
+      <c r="C3" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="81" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="83" t="s">
+      <c r="G3" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="83" t="s">
+      <c r="H3" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="83" t="s">
+      <c r="I3" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="83" t="s">
+      <c r="J3" s="81" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="83" t="s">
+      <c r="K3" s="81" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="84"/>
-      <c r="M3" s="83" t="s">
+      <c r="L3" s="82"/>
+      <c r="M3" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="N3" s="83" t="s">
+      <c r="N3" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="83" t="s">
+      <c r="O3" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="P3" s="83" t="s">
+      <c r="P3" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="83" t="s">
+      <c r="Q3" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="R3" s="83" t="s">
+      <c r="R3" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="S3" s="85" t="s">
+      <c r="S3" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="T3" s="85" t="s">
+      <c r="T3" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="85"/>
-      <c r="V3" s="85"/>
-      <c r="W3" s="85"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="85"/>
-      <c r="Z3" s="85"/>
-      <c r="AA3" s="85"/>
-      <c r="AB3" s="85"/>
-      <c r="AC3" s="85"/>
-      <c r="AD3" s="85"/>
+      <c r="U3" s="83"/>
+      <c r="V3" s="83"/>
+      <c r="W3" s="83"/>
+      <c r="X3" s="83"/>
+      <c r="Y3" s="83"/>
+      <c r="Z3" s="83"/>
+      <c r="AA3" s="83"/>
+      <c r="AB3" s="83"/>
+      <c r="AC3" s="83"/>
+      <c r="AD3" s="83"/>
     </row>
     <row r="4" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="86" t="n">
+      <c r="A4" s="84" t="n">
         <v>42457</v>
       </c>
-      <c r="B4" s="87" t="n">
+      <c r="B4" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C4" s="88" t="n">
+      <c r="C4" s="86" t="n">
         <v>30000</v>
       </c>
-      <c r="D4" s="150" t="n">
+      <c r="D4" s="149" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="151" t="s">
+      <c r="E4" s="150" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="152" t="n">
+      <c r="F4" s="151" t="n">
         <f aca="false">DATEDIF(A4,C18,"Y")</f>
         <v>4</v>
       </c>
-      <c r="G4" s="90" t="n">
+      <c r="G4" s="88" t="n">
         <f aca="false">MAX(0,MIN(48*0.75,DATEDIF(A4,C18,"M")-12))</f>
         <v>36</v>
       </c>
-      <c r="H4" s="91" t="n">
+      <c r="H4" s="89" t="n">
         <f aca="false">C4*0.25+C4*G4/48</f>
         <v>30000</v>
       </c>
-      <c r="I4" s="88" t="n">
+      <c r="I4" s="86" t="n">
         <v>30000</v>
       </c>
-      <c r="J4" s="153" t="n">
+      <c r="J4" s="152" t="n">
         <f aca="false">H4/C4</f>
         <v>1</v>
       </c>
-      <c r="K4" s="86" t="n">
+      <c r="K4" s="84" t="n">
         <f aca="false">DATE(YEAR(A4)+4, MONTH(A4), DAY(A4))</f>
         <v>43918</v>
       </c>
-      <c r="L4" s="93"/>
-      <c r="M4" s="86" t="n">
+      <c r="L4" s="91"/>
+      <c r="M4" s="84" t="n">
         <v>42457</v>
       </c>
-      <c r="N4" s="86" t="n">
+      <c r="N4" s="84" t="n">
         <v>44001</v>
       </c>
-      <c r="O4" s="87" t="n">
+      <c r="O4" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="P4" s="88" t="n">
+      <c r="P4" s="86" t="n">
         <v>30000</v>
       </c>
-      <c r="Q4" s="94" t="n">
+      <c r="Q4" s="92" t="n">
         <f aca="false">P4*O4</f>
         <v>33</v>
       </c>
-      <c r="R4" s="95" t="n">
+      <c r="R4" s="93" t="n">
         <f aca="false">P4*M$1</f>
         <v>75000</v>
       </c>
-      <c r="S4" s="86" t="n">
+      <c r="S4" s="84" t="n">
         <f aca="false">DATE(YEAR(N4)+1,MONTH(N4),DAY(N4))</f>
         <v>44366</v>
       </c>
-      <c r="T4" s="96" t="n">
+      <c r="T4" s="94" t="n">
         <f aca="false">IF($C$18&gt;S4, R4*0.15, R4*0.35)</f>
         <v>26250</v>
       </c>
-      <c r="U4" s="90"/>
-      <c r="V4" s="90"/>
-      <c r="W4" s="90"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="90"/>
-      <c r="Z4" s="90"/>
-      <c r="AA4" s="90"/>
-      <c r="AB4" s="90"/>
-      <c r="AC4" s="90"/>
-      <c r="AD4" s="90"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="88"/>
+      <c r="AB4" s="88"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="88"/>
     </row>
     <row r="5" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="86" t="n">
+      <c r="A5" s="84" t="n">
         <v>43447</v>
       </c>
-      <c r="B5" s="87" t="n">
+      <c r="B5" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C5" s="88" t="n">
+      <c r="C5" s="86" t="n">
         <v>123519</v>
       </c>
-      <c r="D5" s="150" t="n">
+      <c r="D5" s="149" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="151" t="s">
+      <c r="E5" s="150" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="154" t="s">
+      <c r="F5" s="153" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="90" t="n">
+      <c r="G5" s="88" t="n">
         <f aca="false">MAX(0,MIN(36,DATEDIF(A5,C18,"M")))</f>
         <v>18</v>
       </c>
-      <c r="H5" s="91" t="n">
+      <c r="H5" s="89" t="n">
         <f aca="false">C5*0.35+(C5*0.65)*G5/36</f>
         <v>83375.325</v>
       </c>
-      <c r="I5" s="98" t="n">
+      <c r="I5" s="96" t="n">
         <v>83375</v>
       </c>
-      <c r="J5" s="153" t="n">
+      <c r="J5" s="152" t="n">
         <f aca="false">H5/C5</f>
         <v>0.675</v>
       </c>
-      <c r="K5" s="86" t="n">
+      <c r="K5" s="84" t="n">
         <f aca="false">DATE(YEAR(A5)+3, MONTH(A5), DAY(A5))</f>
         <v>44543</v>
       </c>
-      <c r="L5" s="99"/>
-      <c r="M5" s="86" t="n">
+      <c r="L5" s="97"/>
+      <c r="M5" s="84" t="n">
         <v>43447</v>
       </c>
-      <c r="N5" s="86" t="n">
+      <c r="N5" s="84" t="n">
         <v>44001</v>
       </c>
-      <c r="O5" s="87" t="n">
+      <c r="O5" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="P5" s="98" t="n">
+      <c r="P5" s="96" t="n">
         <v>83375</v>
       </c>
-      <c r="Q5" s="94" t="n">
+      <c r="Q5" s="92" t="n">
         <f aca="false">O5*P5</f>
         <v>91.7125</v>
       </c>
-      <c r="R5" s="95" t="n">
+      <c r="R5" s="93" t="n">
         <f aca="false">P5*M$1</f>
         <v>208437.5</v>
       </c>
-      <c r="S5" s="86" t="n">
+      <c r="S5" s="84" t="n">
         <f aca="false">DATE(YEAR(N5)+1,MONTH(N5),DAY(N5))</f>
         <v>44366</v>
       </c>
-      <c r="T5" s="96" t="n">
+      <c r="T5" s="94" t="n">
         <f aca="false">IF($C$18&gt;S5, R5*0.15, R5*0.35)</f>
         <v>72953.125</v>
       </c>
-      <c r="U5" s="90"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="90"/>
-      <c r="Y5" s="90"/>
-      <c r="Z5" s="90"/>
-      <c r="AA5" s="90"/>
-      <c r="AB5" s="90"/>
-      <c r="AC5" s="90"/>
-      <c r="AD5" s="90"/>
+      <c r="U5" s="88"/>
+      <c r="V5" s="88"/>
+      <c r="W5" s="88"/>
+      <c r="X5" s="88"/>
+      <c r="Y5" s="88"/>
+      <c r="Z5" s="88"/>
+      <c r="AA5" s="88"/>
+      <c r="AB5" s="88"/>
+      <c r="AC5" s="88"/>
+      <c r="AD5" s="88"/>
     </row>
     <row r="6" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="86" t="n">
+      <c r="A6" s="84" t="n">
         <v>43602</v>
       </c>
-      <c r="B6" s="87" t="n">
+      <c r="B6" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C6" s="88" t="n">
+      <c r="C6" s="86" t="n">
         <v>38380</v>
       </c>
-      <c r="D6" s="150" t="n">
+      <c r="D6" s="149" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="151" t="s">
+      <c r="E6" s="150" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="152" t="n">
+      <c r="F6" s="151" t="n">
         <f aca="false">DATEDIF(A6,C18,"Y")</f>
         <v>1</v>
       </c>
-      <c r="G6" s="90" t="n">
+      <c r="G6" s="88" t="n">
         <f aca="false">MAX(0,MIN(48*0.75,DATEDIF(A6,C18,"M")-12))</f>
         <v>1</v>
       </c>
-      <c r="H6" s="91" t="n">
+      <c r="H6" s="89" t="n">
         <f aca="false">C6*0.25+C6*G6/48</f>
         <v>10394.5833333333</v>
       </c>
-      <c r="I6" s="98" t="n">
+      <c r="I6" s="96" t="n">
         <v>10394</v>
       </c>
-      <c r="J6" s="153" t="n">
+      <c r="J6" s="152" t="n">
         <f aca="false">H6/C6</f>
         <v>0.270833333333333</v>
       </c>
-      <c r="K6" s="86" t="n">
+      <c r="K6" s="84" t="n">
         <f aca="false">DATE(YEAR(A6)+4, MONTH(A6), DAY(A6))</f>
         <v>45063</v>
       </c>
-      <c r="L6" s="99"/>
-      <c r="M6" s="100" t="n">
+      <c r="L6" s="97"/>
+      <c r="M6" s="98" t="n">
         <v>43602</v>
       </c>
-      <c r="N6" s="100" t="n">
+      <c r="N6" s="98" t="n">
         <v>44001</v>
       </c>
-      <c r="O6" s="101" t="n">
+      <c r="O6" s="99" t="n">
         <v>0.0011</v>
       </c>
-      <c r="P6" s="102" t="n">
+      <c r="P6" s="100" t="n">
         <v>10394</v>
       </c>
-      <c r="Q6" s="103" t="n">
+      <c r="Q6" s="101" t="n">
         <f aca="false">O6*P6</f>
         <v>11.4334</v>
       </c>
-      <c r="R6" s="104" t="n">
+      <c r="R6" s="102" t="n">
         <f aca="false">P6*M$1</f>
         <v>25985</v>
       </c>
-      <c r="S6" s="100" t="n">
+      <c r="S6" s="98" t="n">
         <f aca="false">DATE(YEAR(N6)+1,MONTH(N6),DAY(N6))</f>
         <v>44366</v>
       </c>
-      <c r="T6" s="105" t="n">
+      <c r="T6" s="103" t="n">
         <f aca="false">IF($C$18&gt;S6, R6*0.15, R6*0.35)</f>
         <v>9094.75</v>
       </c>
-      <c r="U6" s="90"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="90"/>
-      <c r="Y6" s="90"/>
-      <c r="Z6" s="90"/>
-      <c r="AA6" s="90"/>
-      <c r="AB6" s="90"/>
-      <c r="AC6" s="90"/>
-      <c r="AD6" s="90"/>
+      <c r="U6" s="88"/>
+      <c r="V6" s="88"/>
+      <c r="W6" s="88"/>
+      <c r="X6" s="88"/>
+      <c r="Y6" s="88"/>
+      <c r="Z6" s="88"/>
+      <c r="AA6" s="88"/>
+      <c r="AB6" s="88"/>
+      <c r="AC6" s="88"/>
+      <c r="AD6" s="88"/>
     </row>
     <row r="7" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="86" t="n">
+      <c r="A7" s="84" t="n">
         <v>43769</v>
       </c>
-      <c r="B7" s="87" t="n">
+      <c r="B7" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="C7" s="88" t="n">
+      <c r="C7" s="86" t="n">
         <v>138965</v>
       </c>
-      <c r="D7" s="150" t="n">
+      <c r="D7" s="149" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="151" t="s">
+      <c r="E7" s="150" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="152" t="n">
+      <c r="F7" s="151" t="n">
         <f aca="false">DATEDIF(A7,C18,"Y")</f>
         <v>0</v>
       </c>
-      <c r="G7" s="90" t="n">
+      <c r="G7" s="88" t="n">
         <f aca="false">MAX(0,MIN(48*0.75,DATEDIF(A7,C18,"M")-12))</f>
         <v>0</v>
       </c>
-      <c r="H7" s="91" t="n">
+      <c r="H7" s="89" t="n">
         <f aca="false">C7*IF(F7&gt;=1,0.25,0)+C7*G7/48</f>
         <v>0</v>
       </c>
-      <c r="I7" s="88" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="153" t="n">
+      <c r="I7" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="152" t="n">
         <f aca="false">H7/C7</f>
         <v>0</v>
       </c>
-      <c r="K7" s="86" t="n">
+      <c r="K7" s="84" t="n">
         <f aca="false">DATE(YEAR(A7)+4, MONTH(A7), DAY(A7))</f>
         <v>45230</v>
       </c>
-      <c r="L7" s="93"/>
-      <c r="M7" s="86" t="n">
+      <c r="L7" s="91"/>
+      <c r="M7" s="84" t="n">
         <v>43447</v>
       </c>
-      <c r="N7" s="108" t="n">
+      <c r="N7" s="106" t="n">
         <v>47848</v>
       </c>
-      <c r="O7" s="87" t="n">
+      <c r="O7" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="P7" s="88" t="n">
+      <c r="P7" s="86" t="n">
         <f aca="false">H5-I5</f>
         <v>0.325000000011642</v>
       </c>
-      <c r="Q7" s="94" t="n">
+      <c r="Q7" s="92" t="n">
         <f aca="false">O7*P7</f>
         <v>0.000357500000012806</v>
       </c>
-      <c r="R7" s="95" t="n">
+      <c r="R7" s="93" t="n">
         <f aca="false">P7*M$1</f>
         <v>0.812500000029104</v>
       </c>
-      <c r="S7" s="86" t="n">
+      <c r="S7" s="84" t="n">
         <f aca="false">DATE(YEAR(N7)+1,MONTH(N7),DAY(N7))</f>
         <v>48213</v>
       </c>
-      <c r="T7" s="96" t="n">
+      <c r="T7" s="94" t="n">
         <f aca="false">IF($C$18&gt;S7, R7*0.15, R7*0.35)</f>
         <v>0.284375000010186</v>
       </c>
-      <c r="U7" s="90"/>
-      <c r="V7" s="90"/>
-      <c r="W7" s="90"/>
-      <c r="X7" s="90"/>
-      <c r="Y7" s="90"/>
-      <c r="Z7" s="90"/>
-      <c r="AA7" s="90"/>
-      <c r="AB7" s="90"/>
-      <c r="AC7" s="90"/>
-      <c r="AD7" s="90"/>
+      <c r="U7" s="88"/>
+      <c r="V7" s="88"/>
+      <c r="W7" s="88"/>
+      <c r="X7" s="88"/>
+      <c r="Y7" s="88"/>
+      <c r="Z7" s="88"/>
+      <c r="AA7" s="88"/>
+      <c r="AB7" s="88"/>
+      <c r="AC7" s="88"/>
+      <c r="AD7" s="88"/>
     </row>
     <row r="8" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="90"/>
-      <c r="B8" s="87"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="150"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="88"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="86" t="n">
+      <c r="A8" s="88"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="149"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="152"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="89"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="88"/>
+      <c r="L8" s="91"/>
+      <c r="M8" s="84" t="n">
         <v>43602</v>
       </c>
-      <c r="N8" s="108" t="n">
+      <c r="N8" s="106" t="n">
         <v>47848</v>
       </c>
-      <c r="O8" s="87" t="n">
+      <c r="O8" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="P8" s="88" t="n">
+      <c r="P8" s="86" t="n">
         <f aca="false">H6-I6</f>
         <v>0.58333333333394</v>
       </c>
-      <c r="Q8" s="94" t="n">
+      <c r="Q8" s="92" t="n">
         <f aca="false">O8*P8</f>
         <v>0.000641666666667334</v>
       </c>
-      <c r="R8" s="95" t="n">
+      <c r="R8" s="93" t="n">
         <f aca="false">P8*M$1</f>
         <v>1.45833333333485</v>
       </c>
-      <c r="S8" s="86" t="n">
+      <c r="S8" s="84" t="n">
         <f aca="false">DATE(YEAR(N8)+1,MONTH(N8),DAY(N8))</f>
         <v>48213</v>
       </c>
-      <c r="T8" s="96" t="n">
+      <c r="T8" s="94" t="n">
         <f aca="false">IF($C$18&gt;S8, R8*0.15, R8*0.35)</f>
         <v>0.510416666667197</v>
       </c>
-      <c r="U8" s="90"/>
-      <c r="V8" s="90"/>
-      <c r="W8" s="90"/>
-      <c r="X8" s="90"/>
-      <c r="Y8" s="90"/>
-      <c r="Z8" s="90"/>
-      <c r="AA8" s="90"/>
-      <c r="AB8" s="90"/>
-      <c r="AC8" s="90"/>
-      <c r="AD8" s="90"/>
+      <c r="U8" s="88"/>
+      <c r="V8" s="88"/>
+      <c r="W8" s="88"/>
+      <c r="X8" s="88"/>
+      <c r="Y8" s="88"/>
+      <c r="Z8" s="88"/>
+      <c r="AA8" s="88"/>
+      <c r="AB8" s="88"/>
+      <c r="AC8" s="88"/>
+      <c r="AD8" s="88"/>
     </row>
     <row r="9" customFormat="false" ht="15.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="90"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="155"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="109"/>
-      <c r="M9" s="86" t="n">
+      <c r="A9" s="88"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="154"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="107"/>
+      <c r="M9" s="84" t="n">
         <v>43769</v>
       </c>
-      <c r="N9" s="108" t="n">
+      <c r="N9" s="106" t="n">
         <v>47848</v>
       </c>
-      <c r="O9" s="87" t="n">
+      <c r="O9" s="85" t="n">
         <v>0.0011</v>
       </c>
-      <c r="P9" s="88" t="n">
+      <c r="P9" s="86" t="n">
         <f aca="false">H7-I7</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="94" t="n">
+      <c r="Q9" s="92" t="n">
         <f aca="false">O9*P9</f>
         <v>0</v>
       </c>
-      <c r="R9" s="95" t="n">
+      <c r="R9" s="93" t="n">
         <f aca="false">P9*M$1</f>
         <v>0</v>
       </c>
-      <c r="S9" s="86" t="n">
+      <c r="S9" s="84" t="n">
         <f aca="false">DATE(YEAR(N9)+1,MONTH(N9),DAY(N9))</f>
         <v>48213</v>
       </c>
-      <c r="T9" s="96" t="n">
+      <c r="T9" s="94" t="n">
         <f aca="false">IF($C$18&gt;S9, R9*0.15, R9*0.35)</f>
         <v>0</v>
       </c>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="90"/>
-      <c r="Y9" s="90"/>
-      <c r="Z9" s="90"/>
-      <c r="AA9" s="90"/>
-      <c r="AB9" s="90"/>
-      <c r="AC9" s="90"/>
-      <c r="AD9" s="90"/>
+      <c r="U9" s="88"/>
+      <c r="V9" s="88"/>
+      <c r="W9" s="88"/>
+      <c r="X9" s="88"/>
+      <c r="Y9" s="88"/>
+      <c r="Z9" s="88"/>
+      <c r="AA9" s="88"/>
+      <c r="AB9" s="88"/>
+      <c r="AC9" s="88"/>
+      <c r="AD9" s="88"/>
     </row>
     <row r="10" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="110"/>
-      <c r="B10" s="90"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="155"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="90"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="109"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="156"/>
-      <c r="O10" s="90"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="94"/>
-      <c r="R10" s="95"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="90"/>
-      <c r="X10" s="90"/>
-      <c r="Y10" s="90"/>
-      <c r="Z10" s="90"/>
-      <c r="AA10" s="90"/>
-      <c r="AB10" s="90"/>
-      <c r="AC10" s="90"/>
-      <c r="AD10" s="90"/>
+      <c r="A10" s="108"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="107"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="155"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="92"/>
+      <c r="R10" s="93"/>
+      <c r="S10" s="88"/>
+      <c r="T10" s="88"/>
+      <c r="U10" s="88"/>
+      <c r="V10" s="88"/>
+      <c r="W10" s="88"/>
+      <c r="X10" s="88"/>
+      <c r="Y10" s="88"/>
+      <c r="Z10" s="88"/>
+      <c r="AA10" s="88"/>
+      <c r="AB10" s="88"/>
+      <c r="AC10" s="88"/>
+      <c r="AD10" s="88"/>
     </row>
     <row r="11" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88"/>
-      <c r="B11" s="90"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="155"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="109"/>
-      <c r="M11" s="90"/>
-      <c r="N11" s="90"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="94"/>
-      <c r="R11" s="95"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="90"/>
-      <c r="V11" s="90"/>
-      <c r="W11" s="90"/>
-      <c r="X11" s="90"/>
-      <c r="Y11" s="90"/>
-      <c r="Z11" s="90"/>
-      <c r="AA11" s="90"/>
-      <c r="AB11" s="90"/>
-      <c r="AC11" s="90"/>
-      <c r="AD11" s="90"/>
+      <c r="A11" s="86"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="154"/>
+      <c r="E11" s="88"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="L11" s="107"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="92"/>
+      <c r="R11" s="93"/>
+      <c r="S11" s="88"/>
+      <c r="T11" s="88"/>
+      <c r="U11" s="88"/>
+      <c r="V11" s="88"/>
+      <c r="W11" s="88"/>
+      <c r="X11" s="88"/>
+      <c r="Y11" s="88"/>
+      <c r="Z11" s="88"/>
+      <c r="AA11" s="88"/>
+      <c r="AB11" s="88"/>
+      <c r="AC11" s="88"/>
+      <c r="AD11" s="88"/>
     </row>
     <row r="12" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="111"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="155"/>
-      <c r="E12" s="90"/>
-      <c r="F12" s="90"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="90"/>
-      <c r="I12" s="90"/>
-      <c r="J12" s="90"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="109"/>
-      <c r="M12" s="90"/>
-      <c r="N12" s="90"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="95"/>
-      <c r="Q12" s="94"/>
-      <c r="R12" s="90"/>
-      <c r="S12" s="90"/>
-      <c r="T12" s="90"/>
-      <c r="U12" s="90"/>
-      <c r="V12" s="90"/>
-      <c r="W12" s="90"/>
-      <c r="X12" s="90"/>
-      <c r="Y12" s="90"/>
-      <c r="Z12" s="90"/>
-      <c r="AA12" s="90"/>
-      <c r="AB12" s="90"/>
-      <c r="AC12" s="90"/>
-      <c r="AD12" s="90"/>
+      <c r="A12" s="109"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="88"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="88"/>
+      <c r="L12" s="107"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="93"/>
+      <c r="Q12" s="92"/>
+      <c r="R12" s="88"/>
+      <c r="S12" s="88"/>
+      <c r="T12" s="88"/>
+      <c r="U12" s="88"/>
+      <c r="V12" s="88"/>
+      <c r="W12" s="88"/>
+      <c r="X12" s="88"/>
+      <c r="Y12" s="88"/>
+      <c r="Z12" s="88"/>
+      <c r="AA12" s="88"/>
+      <c r="AB12" s="88"/>
+      <c r="AC12" s="88"/>
+      <c r="AD12" s="88"/>
     </row>
     <row r="13" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="112"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="85"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="90"/>
-      <c r="F13" s="90"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="85"/>
-      <c r="L13" s="114"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="90"/>
-      <c r="O13" s="90"/>
-      <c r="P13" s="95"/>
-      <c r="Q13" s="94"/>
-      <c r="R13" s="90"/>
-      <c r="S13" s="90"/>
-      <c r="T13" s="90"/>
-      <c r="U13" s="90"/>
-      <c r="V13" s="90"/>
-      <c r="W13" s="90"/>
-      <c r="X13" s="90"/>
-      <c r="Y13" s="90"/>
-      <c r="Z13" s="90"/>
-      <c r="AA13" s="90"/>
-      <c r="AB13" s="90"/>
-      <c r="AC13" s="90"/>
-      <c r="AD13" s="90"/>
+      <c r="A13" s="110"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="83"/>
+      <c r="L13" s="112"/>
+      <c r="M13" s="88"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="92"/>
+      <c r="R13" s="88"/>
+      <c r="S13" s="88"/>
+      <c r="T13" s="88"/>
+      <c r="U13" s="88"/>
+      <c r="V13" s="88"/>
+      <c r="W13" s="88"/>
+      <c r="X13" s="88"/>
+      <c r="Y13" s="88"/>
+      <c r="Z13" s="88"/>
+      <c r="AA13" s="88"/>
+      <c r="AB13" s="88"/>
+      <c r="AC13" s="88"/>
+      <c r="AD13" s="88"/>
     </row>
     <row r="14" customFormat="false" ht="13.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="86"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="150"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="90"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="90"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="90"/>
-      <c r="O14" s="90"/>
-      <c r="P14" s="95"/>
-      <c r="Q14" s="94"/>
-      <c r="R14" s="90"/>
-      <c r="S14" s="90"/>
-      <c r="T14" s="90"/>
-      <c r="U14" s="90"/>
-      <c r="V14" s="90"/>
-      <c r="W14" s="90"/>
-      <c r="X14" s="90"/>
-      <c r="Y14" s="90"/>
-      <c r="Z14" s="90"/>
-      <c r="AA14" s="90"/>
-      <c r="AB14" s="90"/>
-      <c r="AC14" s="90"/>
-      <c r="AD14" s="90"/>
+      <c r="A14" s="84"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="149"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="88"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="92"/>
+      <c r="R14" s="88"/>
+      <c r="S14" s="88"/>
+      <c r="T14" s="88"/>
+      <c r="U14" s="88"/>
+      <c r="V14" s="88"/>
+      <c r="W14" s="88"/>
+      <c r="X14" s="88"/>
+      <c r="Y14" s="88"/>
+      <c r="Z14" s="88"/>
+      <c r="AA14" s="88"/>
+      <c r="AB14" s="88"/>
+      <c r="AC14" s="88"/>
+      <c r="AD14" s="88"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="86"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="109"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
-      <c r="O15" s="90"/>
-      <c r="P15" s="95"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="90"/>
-      <c r="W15" s="90"/>
-      <c r="X15" s="90"/>
-      <c r="Y15" s="90"/>
-      <c r="Z15" s="90"/>
-      <c r="AA15" s="90"/>
-      <c r="AB15" s="90"/>
-      <c r="AC15" s="90"/>
-      <c r="AD15" s="90"/>
-    </row>
-    <row r="16" s="158" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="115" t="str">
+      <c r="A15" s="84"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="149"/>
+      <c r="E15" s="88"/>
+      <c r="F15" s="88"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="88"/>
+      <c r="I15" s="88"/>
+      <c r="J15" s="88"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="107"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="88"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="88"/>
+      <c r="R15" s="88"/>
+      <c r="S15" s="88"/>
+      <c r="T15" s="88"/>
+      <c r="U15" s="88"/>
+      <c r="V15" s="88"/>
+      <c r="W15" s="88"/>
+      <c r="X15" s="88"/>
+      <c r="Y15" s="88"/>
+      <c r="Z15" s="88"/>
+      <c r="AA15" s="88"/>
+      <c r="AB15" s="88"/>
+      <c r="AC15" s="88"/>
+      <c r="AD15" s="88"/>
+    </row>
+    <row r="16" s="157" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="113" t="str">
         <f aca="false">"Grants: "&amp;COUNT(A4:A7)</f>
         <v>Grants: 4</v>
       </c>
-      <c r="B16" s="116"/>
-      <c r="C16" s="117" t="n">
+      <c r="B16" s="114"/>
+      <c r="C16" s="115" t="n">
         <f aca="false">SUM(C4:C7)</f>
         <v>330864</v>
       </c>
-      <c r="D16" s="157"/>
-      <c r="E16" s="117"/>
-      <c r="F16" s="121"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="119" t="n">
+      <c r="D16" s="156"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="119"/>
+      <c r="G16" s="116"/>
+      <c r="H16" s="117" t="n">
         <f aca="false">SUM(H4:H8)</f>
         <v>123769.908333333</v>
       </c>
-      <c r="I16" s="117" t="n">
+      <c r="I16" s="115" t="n">
         <f aca="false">SUM(I4:I8)</f>
         <v>123769</v>
       </c>
-      <c r="J16" s="121" t="n">
+      <c r="J16" s="119" t="n">
         <f aca="false">H16/C16</f>
         <v>0.374080916428905</v>
       </c>
-      <c r="K16" s="121"/>
-      <c r="L16" s="122"/>
-      <c r="M16" s="123" t="s">
+      <c r="K16" s="119"/>
+      <c r="L16" s="120"/>
+      <c r="M16" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="N16" s="123"/>
-      <c r="O16" s="123"/>
-      <c r="P16" s="123"/>
-      <c r="Q16" s="123"/>
-      <c r="R16" s="124" t="n">
+      <c r="N16" s="121"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="121"/>
+      <c r="Q16" s="121"/>
+      <c r="R16" s="122" t="n">
         <f aca="false">SUM(R4:R8)</f>
         <v>309424.770833333</v>
       </c>
-      <c r="S16" s="124"/>
-      <c r="T16" s="124"/>
-      <c r="U16" s="118"/>
-      <c r="V16" s="118"/>
-      <c r="W16" s="118"/>
-      <c r="X16" s="118"/>
-      <c r="Y16" s="118"/>
-      <c r="Z16" s="118"/>
-      <c r="AA16" s="118"/>
-      <c r="AB16" s="118"/>
-      <c r="AC16" s="118"/>
-      <c r="AD16" s="118"/>
-    </row>
-    <row r="17" s="161" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="125"/>
-      <c r="B17" s="126"/>
-      <c r="C17" s="127"/>
-      <c r="D17" s="159"/>
-      <c r="E17" s="127"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="128"/>
-      <c r="H17" s="128"/>
-      <c r="I17" s="128"/>
-      <c r="J17" s="128"/>
-      <c r="K17" s="128"/>
-      <c r="L17" s="130"/>
-      <c r="M17" s="123" t="s">
+      <c r="S16" s="122"/>
+      <c r="T16" s="122"/>
+      <c r="U16" s="116"/>
+      <c r="V16" s="116"/>
+      <c r="W16" s="116"/>
+      <c r="X16" s="116"/>
+      <c r="Y16" s="116"/>
+      <c r="Z16" s="116"/>
+      <c r="AA16" s="116"/>
+      <c r="AB16" s="116"/>
+      <c r="AC16" s="116"/>
+      <c r="AD16" s="116"/>
+    </row>
+    <row r="17" s="160" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="123"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="158"/>
+      <c r="E17" s="125"/>
+      <c r="F17" s="159"/>
+      <c r="G17" s="126"/>
+      <c r="H17" s="126"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="126"/>
+      <c r="K17" s="126"/>
+      <c r="L17" s="128"/>
+      <c r="M17" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="N17" s="123"/>
-      <c r="O17" s="123"/>
-      <c r="P17" s="123"/>
-      <c r="Q17" s="123"/>
-      <c r="R17" s="131" t="n">
+      <c r="N17" s="121"/>
+      <c r="O17" s="121"/>
+      <c r="P17" s="121"/>
+      <c r="Q17" s="121"/>
+      <c r="R17" s="129" t="n">
         <f aca="false">SUM(T4:T9)</f>
         <v>108298.669791667</v>
       </c>
-      <c r="S17" s="131"/>
-      <c r="T17" s="131"/>
-      <c r="U17" s="128"/>
-      <c r="V17" s="128"/>
-      <c r="W17" s="128"/>
-      <c r="X17" s="128"/>
-      <c r="Y17" s="128"/>
-      <c r="Z17" s="128"/>
-      <c r="AA17" s="128"/>
-      <c r="AB17" s="128"/>
-      <c r="AC17" s="128"/>
-      <c r="AD17" s="128"/>
+      <c r="S17" s="129"/>
+      <c r="T17" s="129"/>
+      <c r="U17" s="126"/>
+      <c r="V17" s="126"/>
+      <c r="W17" s="126"/>
+      <c r="X17" s="126"/>
+      <c r="Y17" s="126"/>
+      <c r="Z17" s="126"/>
+      <c r="AA17" s="126"/>
+      <c r="AB17" s="126"/>
+      <c r="AC17" s="126"/>
+      <c r="AD17" s="126"/>
     </row>
     <row r="18" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="86"/>
-      <c r="B18" s="85" t="s">
+      <c r="A18" s="84"/>
+      <c r="B18" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="132" t="n">
+      <c r="C18" s="130" t="n">
         <v>44001</v>
       </c>
-      <c r="D18" s="132"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="153"/>
-      <c r="G18" s="90"/>
-      <c r="H18" s="90"/>
-      <c r="I18" s="90"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="90"/>
-      <c r="M18" s="134" t="s">
+      <c r="D18" s="130"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="152"/>
+      <c r="G18" s="88"/>
+      <c r="H18" s="88"/>
+      <c r="I18" s="88"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="88"/>
+      <c r="L18" s="88"/>
+      <c r="M18" s="132" t="s">
         <v>103</v>
       </c>
-      <c r="N18" s="134"/>
-      <c r="O18" s="134"/>
-      <c r="P18" s="134"/>
-      <c r="Q18" s="134"/>
-      <c r="R18" s="135" t="n">
+      <c r="N18" s="132"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="132"/>
+      <c r="Q18" s="132"/>
+      <c r="R18" s="133" t="n">
         <f aca="false">R16-R17</f>
         <v>201126.101041667</v>
       </c>
-      <c r="S18" s="135"/>
-      <c r="T18" s="135"/>
-      <c r="U18" s="90"/>
-      <c r="V18" s="90"/>
-      <c r="W18" s="90"/>
-      <c r="X18" s="90"/>
-      <c r="Y18" s="90"/>
-      <c r="Z18" s="90"/>
-      <c r="AA18" s="90"/>
-      <c r="AB18" s="90"/>
-      <c r="AC18" s="90"/>
-      <c r="AD18" s="90"/>
+      <c r="S18" s="133"/>
+      <c r="T18" s="133"/>
+      <c r="U18" s="88"/>
+      <c r="V18" s="88"/>
+      <c r="W18" s="88"/>
+      <c r="X18" s="88"/>
+      <c r="Y18" s="88"/>
+      <c r="Z18" s="88"/>
+      <c r="AA18" s="88"/>
+      <c r="AB18" s="88"/>
+      <c r="AC18" s="88"/>
+      <c r="AD18" s="88"/>
     </row>
     <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="86"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="132"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="153"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
-      <c r="J19" s="90"/>
-      <c r="K19" s="90"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="136" t="s">
+      <c r="A19" s="84"/>
+      <c r="B19" s="83"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="152"/>
+      <c r="G19" s="88"/>
+      <c r="H19" s="88"/>
+      <c r="I19" s="88"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="88"/>
+      <c r="L19" s="88"/>
+      <c r="M19" s="134" t="s">
         <v>119</v>
       </c>
-      <c r="N19" s="136"/>
-      <c r="O19" s="136"/>
-      <c r="P19" s="136"/>
-      <c r="Q19" s="136"/>
-      <c r="R19" s="137" t="n">
+      <c r="N19" s="134"/>
+      <c r="O19" s="134"/>
+      <c r="P19" s="134"/>
+      <c r="Q19" s="134"/>
+      <c r="R19" s="135" t="n">
         <f aca="false">(C16-H16)*M1*0.65</f>
         <v>336527.898958333</v>
       </c>
-      <c r="S19" s="137"/>
-      <c r="T19" s="137"/>
-      <c r="U19" s="90"/>
-      <c r="V19" s="90"/>
-      <c r="W19" s="90"/>
-      <c r="X19" s="90"/>
-      <c r="Y19" s="90"/>
-      <c r="Z19" s="90"/>
-      <c r="AA19" s="90"/>
-      <c r="AB19" s="90"/>
-      <c r="AC19" s="90"/>
-      <c r="AD19" s="90"/>
+      <c r="S19" s="135"/>
+      <c r="T19" s="135"/>
+      <c r="U19" s="88"/>
+      <c r="V19" s="88"/>
+      <c r="W19" s="88"/>
+      <c r="X19" s="88"/>
+      <c r="Y19" s="88"/>
+      <c r="Z19" s="88"/>
+      <c r="AA19" s="88"/>
+      <c r="AB19" s="88"/>
+      <c r="AC19" s="88"/>
+      <c r="AD19" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>